<commit_message>
inclusion del modulo de cuentas en factura
</commit_message>
<xml_diff>
--- a/storage/plantillas_excel/Schlumberger Surenco.xlsx
+++ b/storage/plantillas_excel/Schlumberger Surenco.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jtorres\Desktop\XAMPP\htdocs\Psig5.0\storage\plantillas_excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jtorres\Desktop\pruebas\Documentos ecxel\portalsig\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Bogota D.C. - Colombia</t>
   </si>
@@ -115,37 +115,6 @@
   </si>
   <si>
     <t>REEMBOLSO DE   GASTOS    NO GENERADORES DE IVA</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">CONSIGNAR A NOMBRE DE SYSTEM INTEGRAL GROUP S.A.S.  </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">BANCO BBVA CUENTA DE AHORROS </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>497271454</t>
-    </r>
   </si>
   <si>
     <t>INGRESOS EXCLUIDOS DE IVA</t>
@@ -445,7 +414,7 @@
     <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="169" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="118">
+  <cellXfs count="117">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -495,67 +464,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="justify"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="justify"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="justify"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="justify"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="justify"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -635,12 +543,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="10" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -649,12 +551,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -665,15 +561,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -687,12 +574,6 @@
     <xf numFmtId="166" fontId="1" fillId="3" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="167" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -720,6 +601,81 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="justify"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="justify"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="justify"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="justify"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="justify"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Millares 2" xfId="4"/>
@@ -1257,8 +1213,8 @@
   </sheetPr>
   <dimension ref="A1:P48"/>
   <sheetViews>
-    <sheetView showGridLines="0" showZeros="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A10" zoomScale="70" zoomScaleNormal="100" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <selection activeCell="N32" sqref="N32"/>
+    <sheetView showGridLines="0" showZeros="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A9" zoomScale="70" zoomScaleNormal="100" zoomScaleSheetLayoutView="70" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1340,15 +1296,15 @@
       </c>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B5" s="25"/>
-      <c r="C5" s="25"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="25"/>
-      <c r="H5" s="25"/>
-      <c r="I5" s="25"/>
-      <c r="J5" s="25"/>
+      <c r="B5" s="97"/>
+      <c r="C5" s="97"/>
+      <c r="D5" s="97"/>
+      <c r="E5" s="97"/>
+      <c r="F5" s="97"/>
+      <c r="G5" s="97"/>
+      <c r="H5" s="97"/>
+      <c r="I5" s="97"/>
+      <c r="J5" s="97"/>
       <c r="K5" s="9"/>
       <c r="L5" s="9"/>
       <c r="M5" s="8" t="s">
@@ -1356,17 +1312,17 @@
       </c>
     </row>
     <row r="6" spans="2:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="46" t="s">
+      <c r="B6" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="46"/>
-      <c r="D6" s="46"/>
-      <c r="E6" s="46"/>
-      <c r="F6" s="46"/>
-      <c r="G6" s="46"/>
-      <c r="H6" s="46"/>
-      <c r="I6" s="46"/>
-      <c r="J6" s="46"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="25"/>
+      <c r="I6" s="25"/>
+      <c r="J6" s="25"/>
       <c r="K6" s="9"/>
       <c r="L6" s="9"/>
       <c r="M6" s="8" t="s">
@@ -1402,97 +1358,97 @@
       <c r="K8" s="9"/>
       <c r="L8" s="9"/>
       <c r="M8" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B9" s="83"/>
-      <c r="C9" s="84"/>
-      <c r="D9" s="84"/>
-      <c r="E9" s="84"/>
-      <c r="F9" s="84"/>
-      <c r="G9" s="84"/>
-      <c r="H9" s="84"/>
-      <c r="I9" s="84"/>
-      <c r="J9" s="84"/>
-      <c r="K9" s="85"/>
+      <c r="B9" s="60"/>
+      <c r="C9" s="61"/>
+      <c r="D9" s="61"/>
+      <c r="E9" s="61"/>
+      <c r="F9" s="61"/>
+      <c r="G9" s="61"/>
+      <c r="H9" s="61"/>
+      <c r="I9" s="61"/>
+      <c r="J9" s="61"/>
+      <c r="K9" s="62"/>
       <c r="L9" s="4"/>
-      <c r="M9" s="78"/>
+      <c r="M9" s="57"/>
     </row>
     <row r="10" spans="2:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="86" t="s">
+      <c r="B10" s="63" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="47"/>
-      <c r="D10" s="47"/>
-      <c r="E10" s="112"/>
-      <c r="F10" s="112"/>
-      <c r="G10" s="113"/>
-      <c r="H10" s="113"/>
-      <c r="I10" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="J10" s="26"/>
-      <c r="K10" s="114"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="82"/>
+      <c r="F10" s="82"/>
+      <c r="G10" s="83"/>
+      <c r="H10" s="83"/>
+      <c r="I10" s="93" t="s">
+        <v>30</v>
+      </c>
+      <c r="J10" s="93"/>
+      <c r="K10" s="84"/>
       <c r="L10" s="4"/>
-      <c r="M10" s="79" t="s">
+      <c r="M10" s="88" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="11" spans="2:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="87" t="s">
+      <c r="B11" s="90" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="88"/>
-      <c r="D11" s="88"/>
-      <c r="E11" s="48"/>
-      <c r="F11" s="48"/>
-      <c r="G11" s="48"/>
-      <c r="H11" s="48"/>
-      <c r="I11" s="48"/>
-      <c r="J11" s="48"/>
-      <c r="K11" s="89"/>
+      <c r="C11" s="91"/>
+      <c r="D11" s="91"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="27"/>
+      <c r="H11" s="27"/>
+      <c r="I11" s="27"/>
+      <c r="J11" s="27"/>
+      <c r="K11" s="64"/>
       <c r="L11" s="4"/>
-      <c r="M11" s="80"/>
+      <c r="M11" s="89"/>
     </row>
     <row r="12" spans="2:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="86" t="s">
+      <c r="B12" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="49"/>
-      <c r="D12" s="50"/>
-      <c r="E12" s="50"/>
-      <c r="F12" s="50"/>
-      <c r="G12" s="50"/>
-      <c r="H12" s="50"/>
-      <c r="I12" s="50"/>
-      <c r="J12" s="90" t="s">
+      <c r="C12" s="28"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="29"/>
+      <c r="I12" s="29"/>
+      <c r="J12" s="65" t="s">
         <v>16</v>
       </c>
-      <c r="K12" s="115"/>
+      <c r="K12" s="85"/>
       <c r="L12" s="4"/>
-      <c r="M12" s="81"/>
+      <c r="M12" s="58"/>
     </row>
     <row r="13" spans="2:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="28" t="s">
+      <c r="B13" s="92" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="26"/>
-      <c r="D13" s="51"/>
-      <c r="E13" s="48"/>
-      <c r="F13" s="48"/>
-      <c r="G13" s="48"/>
-      <c r="H13" s="48"/>
-      <c r="I13" s="48"/>
-      <c r="J13" s="90" t="s">
+      <c r="C13" s="93"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="27"/>
+      <c r="H13" s="27"/>
+      <c r="I13" s="27"/>
+      <c r="J13" s="65" t="s">
         <v>14</v>
       </c>
-      <c r="K13" s="115"/>
+      <c r="K13" s="85"/>
       <c r="L13" s="4"/>
-      <c r="M13" s="81"/>
+      <c r="M13" s="58"/>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B14" s="86"/>
+      <c r="B14" s="63"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -1501,12 +1457,12 @@
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
-      <c r="K14" s="92"/>
+      <c r="K14" s="67"/>
       <c r="L14" s="4"/>
-      <c r="M14" s="82"/>
+      <c r="M14" s="59"/>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B15" s="93"/>
+      <c r="B15" s="68"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
@@ -1515,208 +1471,208 @@
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
-      <c r="K15" s="94"/>
+      <c r="K15" s="69"/>
       <c r="L15" s="4"/>
       <c r="M15" s="4"/>
     </row>
     <row r="16" spans="2:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="95" t="s">
+      <c r="B16" s="94" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="96"/>
-      <c r="D16" s="96"/>
-      <c r="E16" s="96"/>
-      <c r="F16" s="96"/>
-      <c r="G16" s="96"/>
-      <c r="H16" s="96"/>
-      <c r="I16" s="96"/>
-      <c r="J16" s="97"/>
-      <c r="K16" s="95" t="s">
+      <c r="C16" s="95"/>
+      <c r="D16" s="95"/>
+      <c r="E16" s="95"/>
+      <c r="F16" s="95"/>
+      <c r="G16" s="95"/>
+      <c r="H16" s="95"/>
+      <c r="I16" s="95"/>
+      <c r="J16" s="96"/>
+      <c r="K16" s="94" t="s">
         <v>12</v>
       </c>
-      <c r="L16" s="97"/>
-      <c r="M16" s="91" t="s">
+      <c r="L16" s="96"/>
+      <c r="M16" s="66" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:16" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="15"/>
-      <c r="B17" s="63"/>
-      <c r="C17" s="62"/>
-      <c r="D17" s="62"/>
-      <c r="E17" s="62"/>
-      <c r="F17" s="62"/>
-      <c r="G17" s="62"/>
-      <c r="H17" s="62"/>
-      <c r="I17" s="62"/>
-      <c r="J17" s="62"/>
-      <c r="K17" s="54"/>
-      <c r="L17" s="55"/>
-      <c r="M17" s="61"/>
+      <c r="B17" s="42"/>
+      <c r="C17" s="41"/>
+      <c r="D17" s="41"/>
+      <c r="E17" s="41"/>
+      <c r="F17" s="41"/>
+      <c r="G17" s="41"/>
+      <c r="H17" s="41"/>
+      <c r="I17" s="41"/>
+      <c r="J17" s="41"/>
+      <c r="K17" s="33"/>
+      <c r="L17" s="34"/>
+      <c r="M17" s="40"/>
     </row>
     <row r="18" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="15"/>
-      <c r="B18" s="63"/>
-      <c r="C18" s="62"/>
-      <c r="D18" s="62"/>
-      <c r="E18" s="62"/>
-      <c r="F18" s="62"/>
-      <c r="G18" s="62"/>
-      <c r="H18" s="62"/>
-      <c r="I18" s="62"/>
-      <c r="J18" s="62"/>
-      <c r="K18" s="54"/>
-      <c r="L18" s="55"/>
-      <c r="M18" s="61"/>
+      <c r="B18" s="42"/>
+      <c r="C18" s="41"/>
+      <c r="D18" s="41"/>
+      <c r="E18" s="41"/>
+      <c r="F18" s="41"/>
+      <c r="G18" s="41"/>
+      <c r="H18" s="41"/>
+      <c r="I18" s="41"/>
+      <c r="J18" s="41"/>
+      <c r="K18" s="33"/>
+      <c r="L18" s="34"/>
+      <c r="M18" s="40"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19" s="15"/>
-      <c r="B19" s="63"/>
-      <c r="C19" s="62"/>
-      <c r="D19" s="62"/>
-      <c r="E19" s="62"/>
-      <c r="F19" s="62"/>
-      <c r="G19" s="62"/>
-      <c r="H19" s="62"/>
-      <c r="I19" s="62"/>
-      <c r="J19" s="62"/>
-      <c r="K19" s="54"/>
-      <c r="L19" s="55"/>
-      <c r="M19" s="61"/>
+      <c r="B19" s="42"/>
+      <c r="C19" s="41"/>
+      <c r="D19" s="41"/>
+      <c r="E19" s="41"/>
+      <c r="F19" s="41"/>
+      <c r="G19" s="41"/>
+      <c r="H19" s="41"/>
+      <c r="I19" s="41"/>
+      <c r="J19" s="41"/>
+      <c r="K19" s="33"/>
+      <c r="L19" s="34"/>
+      <c r="M19" s="40"/>
     </row>
     <row r="20" spans="1:16" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="15"/>
-      <c r="B20" s="63"/>
-      <c r="C20" s="62"/>
-      <c r="D20" s="62"/>
-      <c r="E20" s="62"/>
-      <c r="F20" s="62"/>
-      <c r="G20" s="62"/>
-      <c r="H20" s="62"/>
-      <c r="I20" s="62"/>
-      <c r="J20" s="64"/>
-      <c r="K20" s="54"/>
-      <c r="L20" s="55"/>
-      <c r="M20" s="61"/>
+      <c r="B20" s="42"/>
+      <c r="C20" s="41"/>
+      <c r="D20" s="41"/>
+      <c r="E20" s="41"/>
+      <c r="F20" s="41"/>
+      <c r="G20" s="41"/>
+      <c r="H20" s="41"/>
+      <c r="I20" s="41"/>
+      <c r="J20" s="43"/>
+      <c r="K20" s="33"/>
+      <c r="L20" s="34"/>
+      <c r="M20" s="40"/>
     </row>
     <row r="21" spans="1:16" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="15"/>
-      <c r="B21" s="63"/>
-      <c r="C21" s="62"/>
-      <c r="D21" s="62"/>
-      <c r="E21" s="110"/>
-      <c r="F21" s="62"/>
-      <c r="G21" s="62"/>
-      <c r="H21" s="62"/>
-      <c r="I21" s="62"/>
-      <c r="J21" s="64"/>
-      <c r="K21" s="54"/>
-      <c r="L21" s="55"/>
-      <c r="M21" s="61"/>
+      <c r="B21" s="42"/>
+      <c r="C21" s="41"/>
+      <c r="D21" s="41"/>
+      <c r="E21" s="80"/>
+      <c r="F21" s="41"/>
+      <c r="G21" s="41"/>
+      <c r="H21" s="41"/>
+      <c r="I21" s="41"/>
+      <c r="J21" s="43"/>
+      <c r="K21" s="33"/>
+      <c r="L21" s="34"/>
+      <c r="M21" s="40"/>
     </row>
     <row r="22" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="15"/>
-      <c r="B22" s="63"/>
-      <c r="C22" s="62"/>
-      <c r="D22" s="62"/>
-      <c r="E22" s="62"/>
-      <c r="F22" s="62"/>
-      <c r="G22" s="62"/>
-      <c r="H22" s="62"/>
-      <c r="I22" s="62"/>
-      <c r="J22" s="64"/>
-      <c r="K22" s="54"/>
-      <c r="L22" s="55"/>
-      <c r="M22" s="61"/>
+      <c r="B22" s="42"/>
+      <c r="C22" s="41"/>
+      <c r="D22" s="41"/>
+      <c r="E22" s="41"/>
+      <c r="F22" s="41"/>
+      <c r="G22" s="41"/>
+      <c r="H22" s="41"/>
+      <c r="I22" s="41"/>
+      <c r="J22" s="43"/>
+      <c r="K22" s="33"/>
+      <c r="L22" s="34"/>
+      <c r="M22" s="40"/>
     </row>
     <row r="23" spans="1:16" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="15"/>
-      <c r="B23" s="63"/>
-      <c r="C23" s="62"/>
-      <c r="D23" s="62"/>
-      <c r="E23" s="62"/>
-      <c r="F23" s="62"/>
-      <c r="G23" s="62"/>
-      <c r="H23" s="62"/>
-      <c r="I23" s="62"/>
-      <c r="J23" s="62"/>
-      <c r="K23" s="58"/>
-      <c r="L23" s="59"/>
+      <c r="B23" s="42"/>
+      <c r="C23" s="41"/>
+      <c r="D23" s="41"/>
+      <c r="E23" s="41"/>
+      <c r="F23" s="41"/>
+      <c r="G23" s="41"/>
+      <c r="H23" s="41"/>
+      <c r="I23" s="41"/>
+      <c r="J23" s="41"/>
+      <c r="K23" s="37"/>
+      <c r="L23" s="38"/>
       <c r="M23" s="17"/>
     </row>
     <row r="24" spans="1:16" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="15"/>
-      <c r="B24" s="63"/>
-      <c r="C24" s="62"/>
-      <c r="D24" s="62"/>
-      <c r="E24" s="62"/>
-      <c r="F24" s="62"/>
-      <c r="G24" s="62"/>
-      <c r="H24" s="62"/>
-      <c r="I24" s="62"/>
-      <c r="J24" s="62"/>
-      <c r="K24" s="56"/>
-      <c r="L24" s="57"/>
+      <c r="B24" s="42"/>
+      <c r="C24" s="41"/>
+      <c r="D24" s="41"/>
+      <c r="E24" s="41"/>
+      <c r="F24" s="41"/>
+      <c r="G24" s="41"/>
+      <c r="H24" s="41"/>
+      <c r="I24" s="41"/>
+      <c r="J24" s="41"/>
+      <c r="K24" s="35"/>
+      <c r="L24" s="36"/>
       <c r="M24" s="18"/>
     </row>
     <row r="25" spans="1:16" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="65"/>
-      <c r="C25" s="66"/>
-      <c r="D25" s="66"/>
-      <c r="E25" s="66"/>
-      <c r="F25" s="66"/>
-      <c r="G25" s="66"/>
-      <c r="H25" s="66"/>
-      <c r="I25" s="66"/>
-      <c r="J25" s="66"/>
-      <c r="K25" s="58"/>
-      <c r="L25" s="59"/>
-      <c r="M25" s="111"/>
+      <c r="B25" s="44"/>
+      <c r="C25" s="45"/>
+      <c r="D25" s="45"/>
+      <c r="E25" s="45"/>
+      <c r="F25" s="45"/>
+      <c r="G25" s="45"/>
+      <c r="H25" s="45"/>
+      <c r="I25" s="45"/>
+      <c r="J25" s="45"/>
+      <c r="K25" s="37"/>
+      <c r="L25" s="38"/>
+      <c r="M25" s="81"/>
     </row>
     <row r="26" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="67"/>
-      <c r="C26" s="68"/>
-      <c r="D26" s="52"/>
-      <c r="E26" s="52"/>
-      <c r="F26" s="52"/>
-      <c r="G26" s="52"/>
-      <c r="H26" s="52"/>
-      <c r="I26" s="69"/>
-      <c r="J26" s="69"/>
-      <c r="K26" s="58"/>
-      <c r="L26" s="59"/>
+      <c r="B26" s="46"/>
+      <c r="C26" s="47"/>
+      <c r="D26" s="31"/>
+      <c r="E26" s="31"/>
+      <c r="F26" s="31"/>
+      <c r="G26" s="31"/>
+      <c r="H26" s="31"/>
+      <c r="I26" s="48"/>
+      <c r="J26" s="48"/>
+      <c r="K26" s="37"/>
+      <c r="L26" s="38"/>
       <c r="M26" s="17"/>
     </row>
     <row r="27" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="65"/>
-      <c r="C27" s="69"/>
-      <c r="D27" s="69"/>
-      <c r="E27" s="69"/>
-      <c r="F27" s="69"/>
-      <c r="G27" s="69"/>
-      <c r="H27" s="69"/>
-      <c r="I27" s="69"/>
-      <c r="J27" s="69"/>
-      <c r="K27" s="58"/>
-      <c r="L27" s="59"/>
+      <c r="B27" s="44"/>
+      <c r="C27" s="48"/>
+      <c r="D27" s="48"/>
+      <c r="E27" s="48"/>
+      <c r="F27" s="48"/>
+      <c r="G27" s="48"/>
+      <c r="H27" s="48"/>
+      <c r="I27" s="48"/>
+      <c r="J27" s="48"/>
+      <c r="K27" s="37"/>
+      <c r="L27" s="38"/>
       <c r="M27" s="17"/>
     </row>
     <row r="28" spans="1:16" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="70"/>
-      <c r="C28" s="71"/>
-      <c r="D28" s="71"/>
-      <c r="E28" s="71"/>
-      <c r="F28" s="71"/>
-      <c r="G28" s="71"/>
-      <c r="H28" s="71"/>
-      <c r="I28" s="71"/>
-      <c r="J28" s="71"/>
-      <c r="K28" s="60"/>
-      <c r="L28" s="102"/>
+      <c r="B28" s="49"/>
+      <c r="C28" s="50"/>
+      <c r="D28" s="50"/>
+      <c r="E28" s="50"/>
+      <c r="F28" s="50"/>
+      <c r="G28" s="50"/>
+      <c r="H28" s="50"/>
+      <c r="I28" s="50"/>
+      <c r="J28" s="50"/>
+      <c r="K28" s="39"/>
+      <c r="L28" s="74"/>
       <c r="M28" s="17"/>
     </row>
     <row r="29" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="53"/>
+      <c r="B29" s="32"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
@@ -1728,8 +1684,8 @@
       <c r="K29" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="L29" s="116"/>
-      <c r="M29" s="99"/>
+      <c r="L29" s="86"/>
+      <c r="M29" s="71"/>
     </row>
     <row r="30" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="19"/>
@@ -1742,119 +1698,117 @@
       <c r="I30" s="3"/>
       <c r="J30" s="16"/>
       <c r="K30" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="L30" s="116"/>
-      <c r="M30" s="99"/>
+        <v>29</v>
+      </c>
+      <c r="L30" s="86"/>
+      <c r="M30" s="71"/>
     </row>
     <row r="31" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="34" t="s">
-        <v>29</v>
-      </c>
-      <c r="C31" s="35"/>
-      <c r="D31" s="35"/>
-      <c r="E31" s="35"/>
-      <c r="F31" s="35"/>
-      <c r="G31" s="35"/>
-      <c r="H31" s="35"/>
-      <c r="I31" s="35"/>
-      <c r="J31" s="36"/>
-      <c r="K31" s="40" t="s">
+      <c r="B31" s="112"/>
+      <c r="C31" s="113"/>
+      <c r="D31" s="113"/>
+      <c r="E31" s="113"/>
+      <c r="F31" s="113"/>
+      <c r="G31" s="113"/>
+      <c r="H31" s="113"/>
+      <c r="I31" s="113"/>
+      <c r="J31" s="114"/>
+      <c r="K31" s="104" t="s">
         <v>28</v>
       </c>
-      <c r="L31" s="77"/>
-      <c r="M31" s="100"/>
+      <c r="L31" s="56"/>
+      <c r="M31" s="72"/>
     </row>
     <row r="32" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="15"/>
-      <c r="B32" s="37"/>
-      <c r="C32" s="38"/>
-      <c r="D32" s="38"/>
-      <c r="E32" s="38"/>
-      <c r="F32" s="38"/>
-      <c r="G32" s="38"/>
-      <c r="H32" s="38"/>
-      <c r="I32" s="38"/>
-      <c r="J32" s="39"/>
-      <c r="K32" s="41"/>
+      <c r="B32" s="115"/>
+      <c r="C32" s="30"/>
+      <c r="D32" s="30"/>
+      <c r="E32" s="30"/>
+      <c r="F32" s="30"/>
+      <c r="G32" s="30"/>
+      <c r="H32" s="30"/>
+      <c r="I32" s="30"/>
+      <c r="J32" s="116"/>
+      <c r="K32" s="105"/>
       <c r="L32" s="24"/>
-      <c r="M32" s="101"/>
+      <c r="M32" s="73"/>
       <c r="P32" s="14"/>
     </row>
     <row r="33" spans="2:16" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="73"/>
-      <c r="C33" s="74"/>
-      <c r="D33" s="74"/>
-      <c r="E33" s="74"/>
-      <c r="F33" s="74"/>
-      <c r="G33" s="74"/>
-      <c r="H33" s="74"/>
-      <c r="I33" s="74"/>
-      <c r="J33" s="75"/>
+      <c r="B33" s="52"/>
+      <c r="C33" s="53"/>
+      <c r="D33" s="53"/>
+      <c r="E33" s="53"/>
+      <c r="F33" s="53"/>
+      <c r="G33" s="53"/>
+      <c r="H33" s="53"/>
+      <c r="I33" s="53"/>
+      <c r="J33" s="54"/>
       <c r="K33" s="21" t="s">
         <v>9</v>
       </c>
       <c r="L33" s="22"/>
-      <c r="M33" s="103">
+      <c r="M33" s="75">
         <f>SUM(M29:M32)</f>
         <v>0</v>
       </c>
       <c r="P33" s="13"/>
     </row>
     <row r="34" spans="2:16" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B34" s="76"/>
-      <c r="C34" s="72"/>
-      <c r="D34" s="72"/>
-      <c r="E34" s="72"/>
-      <c r="F34" s="72"/>
-      <c r="G34" s="72"/>
-      <c r="H34" s="72"/>
-      <c r="I34" s="72"/>
-      <c r="J34" s="72"/>
-      <c r="K34" s="108" t="s">
+      <c r="B34" s="55"/>
+      <c r="C34" s="51"/>
+      <c r="D34" s="51"/>
+      <c r="E34" s="51"/>
+      <c r="F34" s="51"/>
+      <c r="G34" s="51"/>
+      <c r="H34" s="51"/>
+      <c r="I34" s="51"/>
+      <c r="J34" s="51"/>
+      <c r="K34" s="78" t="s">
         <v>8</v>
       </c>
       <c r="L34" s="22"/>
-      <c r="M34" s="106"/>
-      <c r="O34" s="104"/>
-      <c r="P34" s="105"/>
+      <c r="M34" s="76"/>
+      <c r="O34" s="106"/>
+      <c r="P34" s="98"/>
     </row>
     <row r="35" spans="2:16" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B35" s="29" t="s">
+      <c r="B35" s="99" t="s">
         <v>7</v>
       </c>
-      <c r="C35" s="30"/>
-      <c r="D35" s="30"/>
-      <c r="E35" s="30"/>
-      <c r="F35" s="30"/>
-      <c r="G35" s="30"/>
-      <c r="H35" s="30"/>
-      <c r="I35" s="30"/>
-      <c r="J35" s="30"/>
-      <c r="K35" s="109"/>
-      <c r="L35" s="117"/>
-      <c r="M35" s="107"/>
-      <c r="O35" s="104"/>
-      <c r="P35" s="105"/>
+      <c r="C35" s="100"/>
+      <c r="D35" s="100"/>
+      <c r="E35" s="100"/>
+      <c r="F35" s="100"/>
+      <c r="G35" s="100"/>
+      <c r="H35" s="100"/>
+      <c r="I35" s="100"/>
+      <c r="J35" s="100"/>
+      <c r="K35" s="79"/>
+      <c r="L35" s="87"/>
+      <c r="M35" s="77"/>
+      <c r="O35" s="106"/>
+      <c r="P35" s="98"/>
     </row>
     <row r="36" spans="2:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B36" s="31"/>
-      <c r="C36" s="32"/>
-      <c r="D36" s="32"/>
-      <c r="E36" s="32"/>
-      <c r="F36" s="32"/>
-      <c r="G36" s="32"/>
-      <c r="H36" s="32"/>
-      <c r="I36" s="32"/>
-      <c r="J36" s="33"/>
+      <c r="B36" s="101"/>
+      <c r="C36" s="102"/>
+      <c r="D36" s="102"/>
+      <c r="E36" s="102"/>
+      <c r="F36" s="102"/>
+      <c r="G36" s="102"/>
+      <c r="H36" s="102"/>
+      <c r="I36" s="102"/>
+      <c r="J36" s="103"/>
       <c r="K36" s="6" t="s">
         <v>6</v>
       </c>
       <c r="L36" s="23"/>
-      <c r="M36" s="101"/>
+      <c r="M36" s="73"/>
     </row>
     <row r="37" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B37" s="98" t="s">
+      <c r="B37" s="70" t="s">
         <v>5</v>
       </c>
       <c r="C37" s="5"/>
@@ -1864,7 +1818,7 @@
       <c r="G37" s="5"/>
       <c r="H37" s="5"/>
       <c r="I37" s="5"/>
-      <c r="J37" s="94"/>
+      <c r="J37" s="69"/>
       <c r="K37" s="4"/>
       <c r="L37" s="4"/>
       <c r="M37" s="4"/>
@@ -1940,24 +1894,24 @@
       <c r="M42" s="5"/>
     </row>
     <row r="43" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B43" s="42" t="s">
+      <c r="B43" s="108" t="s">
         <v>4</v>
       </c>
-      <c r="C43" s="42"/>
-      <c r="D43" s="42"/>
-      <c r="E43" s="42"/>
-      <c r="F43" s="42"/>
+      <c r="C43" s="108"/>
+      <c r="D43" s="108"/>
+      <c r="E43" s="108"/>
+      <c r="F43" s="108"/>
       <c r="G43" s="4"/>
-      <c r="H43" s="43" t="s">
+      <c r="H43" s="109" t="s">
         <v>3</v>
       </c>
-      <c r="I43" s="43"/>
-      <c r="J43" s="43"/>
+      <c r="I43" s="109"/>
+      <c r="J43" s="109"/>
       <c r="K43" s="3"/>
-      <c r="L43" s="44" t="s">
+      <c r="L43" s="110" t="s">
         <v>2</v>
       </c>
-      <c r="M43" s="44"/>
+      <c r="M43" s="110"/>
       <c r="N43" s="12"/>
       <c r="O43" s="12"/>
       <c r="P43" s="12"/>
@@ -1969,77 +1923,77 @@
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
       <c r="G44" s="2"/>
-      <c r="H44" s="43"/>
-      <c r="I44" s="43"/>
-      <c r="J44" s="43"/>
+      <c r="H44" s="109"/>
+      <c r="I44" s="109"/>
+      <c r="J44" s="109"/>
       <c r="K44" s="1"/>
       <c r="L44" s="1"/>
       <c r="M44" s="1"/>
     </row>
     <row r="45" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B45" s="45"/>
-      <c r="C45" s="45"/>
-      <c r="D45" s="45"/>
-      <c r="E45" s="45"/>
-      <c r="F45" s="45"/>
-      <c r="G45" s="45"/>
-      <c r="H45" s="45"/>
-      <c r="I45" s="45"/>
-      <c r="J45" s="45"/>
-      <c r="K45" s="45"/>
-      <c r="L45" s="45"/>
-      <c r="M45" s="45"/>
+      <c r="B45" s="111"/>
+      <c r="C45" s="111"/>
+      <c r="D45" s="111"/>
+      <c r="E45" s="111"/>
+      <c r="F45" s="111"/>
+      <c r="G45" s="111"/>
+      <c r="H45" s="111"/>
+      <c r="I45" s="111"/>
+      <c r="J45" s="111"/>
+      <c r="K45" s="111"/>
+      <c r="L45" s="111"/>
+      <c r="M45" s="111"/>
     </row>
     <row r="46" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B46" s="27" t="s">
+      <c r="B46" s="107" t="s">
         <v>27</v>
       </c>
-      <c r="C46" s="27"/>
-      <c r="D46" s="27"/>
-      <c r="E46" s="27"/>
-      <c r="F46" s="27"/>
-      <c r="G46" s="27"/>
-      <c r="H46" s="27"/>
-      <c r="I46" s="27"/>
-      <c r="J46" s="27"/>
-      <c r="K46" s="27"/>
-      <c r="L46" s="27"/>
-      <c r="M46" s="27"/>
+      <c r="C46" s="107"/>
+      <c r="D46" s="107"/>
+      <c r="E46" s="107"/>
+      <c r="F46" s="107"/>
+      <c r="G46" s="107"/>
+      <c r="H46" s="107"/>
+      <c r="I46" s="107"/>
+      <c r="J46" s="107"/>
+      <c r="K46" s="107"/>
+      <c r="L46" s="107"/>
+      <c r="M46" s="107"/>
     </row>
     <row r="47" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B47" s="27" t="s">
+      <c r="B47" s="107" t="s">
         <v>1</v>
       </c>
-      <c r="C47" s="27"/>
-      <c r="D47" s="27"/>
-      <c r="E47" s="27"/>
-      <c r="F47" s="27"/>
-      <c r="G47" s="27"/>
-      <c r="H47" s="27"/>
-      <c r="I47" s="27"/>
-      <c r="J47" s="27"/>
-      <c r="K47" s="27"/>
-      <c r="L47" s="27"/>
-      <c r="M47" s="27"/>
+      <c r="C47" s="107"/>
+      <c r="D47" s="107"/>
+      <c r="E47" s="107"/>
+      <c r="F47" s="107"/>
+      <c r="G47" s="107"/>
+      <c r="H47" s="107"/>
+      <c r="I47" s="107"/>
+      <c r="J47" s="107"/>
+      <c r="K47" s="107"/>
+      <c r="L47" s="107"/>
+      <c r="M47" s="107"/>
     </row>
     <row r="48" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B48" s="27" t="s">
+      <c r="B48" s="107" t="s">
         <v>0</v>
       </c>
-      <c r="C48" s="27"/>
-      <c r="D48" s="27"/>
-      <c r="E48" s="27"/>
-      <c r="F48" s="27"/>
-      <c r="G48" s="27"/>
-      <c r="H48" s="27"/>
-      <c r="I48" s="27"/>
-      <c r="J48" s="27"/>
-      <c r="K48" s="27"/>
-      <c r="L48" s="27"/>
-      <c r="M48" s="27"/>
+      <c r="C48" s="107"/>
+      <c r="D48" s="107"/>
+      <c r="E48" s="107"/>
+      <c r="F48" s="107"/>
+      <c r="G48" s="107"/>
+      <c r="H48" s="107"/>
+      <c r="I48" s="107"/>
+      <c r="J48" s="107"/>
+      <c r="K48" s="107"/>
+      <c r="L48" s="107"/>
+      <c r="M48" s="107"/>
     </row>
   </sheetData>
-  <mergeCells count="19">
+  <mergeCells count="18">
     <mergeCell ref="B48:M48"/>
     <mergeCell ref="B43:F43"/>
     <mergeCell ref="H43:J44"/>
@@ -2047,18 +2001,17 @@
     <mergeCell ref="B45:M45"/>
     <mergeCell ref="B46:M46"/>
     <mergeCell ref="B47:M47"/>
+    <mergeCell ref="B5:J5"/>
+    <mergeCell ref="I10:J10"/>
     <mergeCell ref="P34:P35"/>
     <mergeCell ref="B35:J36"/>
-    <mergeCell ref="B31:J32"/>
     <mergeCell ref="K31:K32"/>
     <mergeCell ref="O34:O35"/>
+    <mergeCell ref="M10:M11"/>
+    <mergeCell ref="B11:D11"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="B16:J16"/>
     <mergeCell ref="K16:L16"/>
-    <mergeCell ref="B5:J5"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="M10:M11"/>
-    <mergeCell ref="B11:D11"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
arreglos en descarga excel
</commit_message>
<xml_diff>
--- a/storage/plantillas_excel/Schlumberger Surenco.xlsx
+++ b/storage/plantillas_excel/Schlumberger Surenco.xlsx
@@ -130,14 +130,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="7">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;\ #,##0"/>
-    <numFmt numFmtId="165" formatCode="&quot;$&quot;\ #,##0.00;&quot;$&quot;\ \-#,##0.00"/>
-    <numFmt numFmtId="166" formatCode="&quot;$&quot;\ #,##0;&quot;$&quot;\ \-#,##0"/>
     <numFmt numFmtId="167" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="168" formatCode="_ &quot;$&quot;\ * #,##0.00_ ;_ &quot;$&quot;\ * \-#,##0.00_ ;_ &quot;$&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="169" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="170" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="171" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
   <fonts count="15" x14ac:knownFonts="1">
     <font>
@@ -474,21 +472,6 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="170" fontId="1" fillId="3" borderId="12" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="1" fillId="3" borderId="3" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="1" fillId="3" borderId="12" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="170" fontId="1" fillId="3" borderId="3" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="1" fillId="3" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="1" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -571,7 +554,6 @@
     <xf numFmtId="164" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="3" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -600,82 +582,98 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="justify"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="justify"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="justify"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="justify"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="justify"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="justify"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="justify"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="justify"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="justify"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="justify"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="1" fillId="3" borderId="12" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="1" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="171" fontId="1" fillId="3" borderId="12" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="171" fontId="1" fillId="3" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="4" fontId="1" fillId="3" borderId="3" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="4" fontId="1" fillId="3" borderId="3" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="3" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Millares 2" xfId="4"/>
@@ -1213,8 +1211,8 @@
   </sheetPr>
   <dimension ref="A1:P48"/>
   <sheetViews>
-    <sheetView showGridLines="0" showZeros="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A9" zoomScale="70" zoomScaleNormal="100" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView showGridLines="0" showZeros="0" tabSelected="1" view="pageBreakPreview" zoomScale="70" zoomScaleNormal="100" zoomScaleSheetLayoutView="70" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1296,15 +1294,15 @@
       </c>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B5" s="97"/>
-      <c r="C5" s="97"/>
-      <c r="D5" s="97"/>
-      <c r="E5" s="97"/>
-      <c r="F5" s="97"/>
-      <c r="G5" s="97"/>
-      <c r="H5" s="97"/>
-      <c r="I5" s="97"/>
-      <c r="J5" s="97"/>
+      <c r="B5" s="85"/>
+      <c r="C5" s="85"/>
+      <c r="D5" s="85"/>
+      <c r="E5" s="85"/>
+      <c r="F5" s="85"/>
+      <c r="G5" s="85"/>
+      <c r="H5" s="85"/>
+      <c r="I5" s="85"/>
+      <c r="J5" s="85"/>
       <c r="K5" s="9"/>
       <c r="L5" s="9"/>
       <c r="M5" s="8" t="s">
@@ -1362,57 +1360,57 @@
       </c>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B9" s="60"/>
-      <c r="C9" s="61"/>
-      <c r="D9" s="61"/>
-      <c r="E9" s="61"/>
-      <c r="F9" s="61"/>
-      <c r="G9" s="61"/>
-      <c r="H9" s="61"/>
-      <c r="I9" s="61"/>
-      <c r="J9" s="61"/>
-      <c r="K9" s="62"/>
+      <c r="B9" s="53"/>
+      <c r="C9" s="54"/>
+      <c r="D9" s="54"/>
+      <c r="E9" s="54"/>
+      <c r="F9" s="54"/>
+      <c r="G9" s="54"/>
+      <c r="H9" s="54"/>
+      <c r="I9" s="54"/>
+      <c r="J9" s="54"/>
+      <c r="K9" s="55"/>
       <c r="L9" s="4"/>
-      <c r="M9" s="57"/>
+      <c r="M9" s="50"/>
     </row>
     <row r="10" spans="2:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="63" t="s">
+      <c r="B10" s="56" t="s">
         <v>20</v>
       </c>
       <c r="C10" s="26"/>
       <c r="D10" s="26"/>
-      <c r="E10" s="82"/>
-      <c r="F10" s="82"/>
-      <c r="G10" s="83"/>
-      <c r="H10" s="83"/>
-      <c r="I10" s="93" t="s">
+      <c r="E10" s="74"/>
+      <c r="F10" s="74"/>
+      <c r="G10" s="75"/>
+      <c r="H10" s="75"/>
+      <c r="I10" s="86" t="s">
         <v>30</v>
       </c>
-      <c r="J10" s="93"/>
-      <c r="K10" s="84"/>
+      <c r="J10" s="86"/>
+      <c r="K10" s="76"/>
       <c r="L10" s="4"/>
-      <c r="M10" s="88" t="s">
+      <c r="M10" s="96" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="11" spans="2:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="90" t="s">
+      <c r="B11" s="98" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="91"/>
-      <c r="D11" s="91"/>
+      <c r="C11" s="99"/>
+      <c r="D11" s="99"/>
       <c r="E11" s="27"/>
       <c r="F11" s="27"/>
       <c r="G11" s="27"/>
       <c r="H11" s="27"/>
       <c r="I11" s="27"/>
       <c r="J11" s="27"/>
-      <c r="K11" s="64"/>
+      <c r="K11" s="57"/>
       <c r="L11" s="4"/>
-      <c r="M11" s="89"/>
+      <c r="M11" s="97"/>
     </row>
     <row r="12" spans="2:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="63" t="s">
+      <c r="B12" s="56" t="s">
         <v>17</v>
       </c>
       <c r="C12" s="28"/>
@@ -1422,33 +1420,33 @@
       <c r="G12" s="29"/>
       <c r="H12" s="29"/>
       <c r="I12" s="29"/>
-      <c r="J12" s="65" t="s">
+      <c r="J12" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="K12" s="85"/>
+      <c r="K12" s="77"/>
       <c r="L12" s="4"/>
-      <c r="M12" s="58"/>
+      <c r="M12" s="51"/>
     </row>
     <row r="13" spans="2:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="92" t="s">
+      <c r="B13" s="100" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="93"/>
+      <c r="C13" s="86"/>
       <c r="D13" s="30"/>
       <c r="E13" s="27"/>
       <c r="F13" s="27"/>
       <c r="G13" s="27"/>
       <c r="H13" s="27"/>
       <c r="I13" s="27"/>
-      <c r="J13" s="65" t="s">
+      <c r="J13" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="K13" s="85"/>
+      <c r="K13" s="77"/>
       <c r="L13" s="4"/>
-      <c r="M13" s="58"/>
+      <c r="M13" s="51"/>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B14" s="63"/>
+      <c r="B14" s="56"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -1457,12 +1455,12 @@
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
-      <c r="K14" s="67"/>
+      <c r="K14" s="60"/>
       <c r="L14" s="4"/>
-      <c r="M14" s="59"/>
+      <c r="M14" s="52"/>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B15" s="68"/>
+      <c r="B15" s="61"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
@@ -1471,204 +1469,204 @@
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
-      <c r="K15" s="69"/>
+      <c r="K15" s="62"/>
       <c r="L15" s="4"/>
       <c r="M15" s="4"/>
     </row>
     <row r="16" spans="2:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="94" t="s">
+      <c r="B16" s="101" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="95"/>
-      <c r="D16" s="95"/>
-      <c r="E16" s="95"/>
-      <c r="F16" s="95"/>
-      <c r="G16" s="95"/>
-      <c r="H16" s="95"/>
-      <c r="I16" s="95"/>
-      <c r="J16" s="96"/>
-      <c r="K16" s="94" t="s">
+      <c r="C16" s="102"/>
+      <c r="D16" s="102"/>
+      <c r="E16" s="102"/>
+      <c r="F16" s="102"/>
+      <c r="G16" s="102"/>
+      <c r="H16" s="102"/>
+      <c r="I16" s="102"/>
+      <c r="J16" s="103"/>
+      <c r="K16" s="101" t="s">
         <v>12</v>
       </c>
-      <c r="L16" s="96"/>
-      <c r="M16" s="66" t="s">
+      <c r="L16" s="103"/>
+      <c r="M16" s="59" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:16" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="15"/>
-      <c r="B17" s="42"/>
-      <c r="C17" s="41"/>
-      <c r="D17" s="41"/>
-      <c r="E17" s="41"/>
-      <c r="F17" s="41"/>
-      <c r="G17" s="41"/>
-      <c r="H17" s="41"/>
-      <c r="I17" s="41"/>
-      <c r="J17" s="41"/>
-      <c r="K17" s="33"/>
-      <c r="L17" s="34"/>
-      <c r="M17" s="40"/>
+      <c r="B17" s="35"/>
+      <c r="C17" s="34"/>
+      <c r="D17" s="34"/>
+      <c r="E17" s="34"/>
+      <c r="F17" s="34"/>
+      <c r="G17" s="34"/>
+      <c r="H17" s="34"/>
+      <c r="I17" s="34"/>
+      <c r="J17" s="34"/>
+      <c r="K17" s="109"/>
+      <c r="L17" s="113"/>
+      <c r="M17" s="33"/>
     </row>
     <row r="18" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="15"/>
-      <c r="B18" s="42"/>
-      <c r="C18" s="41"/>
-      <c r="D18" s="41"/>
-      <c r="E18" s="41"/>
-      <c r="F18" s="41"/>
-      <c r="G18" s="41"/>
-      <c r="H18" s="41"/>
-      <c r="I18" s="41"/>
-      <c r="J18" s="41"/>
-      <c r="K18" s="33"/>
-      <c r="L18" s="34"/>
-      <c r="M18" s="40"/>
+      <c r="B18" s="35"/>
+      <c r="C18" s="34"/>
+      <c r="D18" s="34"/>
+      <c r="E18" s="34"/>
+      <c r="F18" s="34"/>
+      <c r="G18" s="34"/>
+      <c r="H18" s="34"/>
+      <c r="I18" s="34"/>
+      <c r="J18" s="34"/>
+      <c r="K18" s="109"/>
+      <c r="L18" s="113"/>
+      <c r="M18" s="33"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19" s="15"/>
-      <c r="B19" s="42"/>
-      <c r="C19" s="41"/>
-      <c r="D19" s="41"/>
-      <c r="E19" s="41"/>
-      <c r="F19" s="41"/>
-      <c r="G19" s="41"/>
-      <c r="H19" s="41"/>
-      <c r="I19" s="41"/>
-      <c r="J19" s="41"/>
-      <c r="K19" s="33"/>
-      <c r="L19" s="34"/>
-      <c r="M19" s="40"/>
+      <c r="B19" s="35"/>
+      <c r="C19" s="34"/>
+      <c r="D19" s="34"/>
+      <c r="E19" s="34"/>
+      <c r="F19" s="34"/>
+      <c r="G19" s="34"/>
+      <c r="H19" s="34"/>
+      <c r="I19" s="34"/>
+      <c r="J19" s="34"/>
+      <c r="K19" s="109"/>
+      <c r="L19" s="113"/>
+      <c r="M19" s="33"/>
     </row>
     <row r="20" spans="1:16" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="15"/>
-      <c r="B20" s="42"/>
-      <c r="C20" s="41"/>
-      <c r="D20" s="41"/>
-      <c r="E20" s="41"/>
-      <c r="F20" s="41"/>
-      <c r="G20" s="41"/>
-      <c r="H20" s="41"/>
-      <c r="I20" s="41"/>
-      <c r="J20" s="43"/>
-      <c r="K20" s="33"/>
-      <c r="L20" s="34"/>
-      <c r="M20" s="40"/>
+      <c r="B20" s="35"/>
+      <c r="C20" s="34"/>
+      <c r="D20" s="34"/>
+      <c r="E20" s="34"/>
+      <c r="F20" s="34"/>
+      <c r="G20" s="34"/>
+      <c r="H20" s="34"/>
+      <c r="I20" s="34"/>
+      <c r="J20" s="36"/>
+      <c r="K20" s="109"/>
+      <c r="L20" s="113"/>
+      <c r="M20" s="33"/>
     </row>
     <row r="21" spans="1:16" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="15"/>
-      <c r="B21" s="42"/>
-      <c r="C21" s="41"/>
-      <c r="D21" s="41"/>
-      <c r="E21" s="80"/>
-      <c r="F21" s="41"/>
-      <c r="G21" s="41"/>
-      <c r="H21" s="41"/>
-      <c r="I21" s="41"/>
-      <c r="J21" s="43"/>
-      <c r="K21" s="33"/>
-      <c r="L21" s="34"/>
-      <c r="M21" s="40"/>
+      <c r="B21" s="35"/>
+      <c r="C21" s="34"/>
+      <c r="D21" s="34"/>
+      <c r="E21" s="72"/>
+      <c r="F21" s="34"/>
+      <c r="G21" s="34"/>
+      <c r="H21" s="34"/>
+      <c r="I21" s="34"/>
+      <c r="J21" s="36"/>
+      <c r="K21" s="109"/>
+      <c r="L21" s="113"/>
+      <c r="M21" s="33"/>
     </row>
     <row r="22" spans="1:16" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="15"/>
-      <c r="B22" s="42"/>
-      <c r="C22" s="41"/>
-      <c r="D22" s="41"/>
-      <c r="E22" s="41"/>
-      <c r="F22" s="41"/>
-      <c r="G22" s="41"/>
-      <c r="H22" s="41"/>
-      <c r="I22" s="41"/>
-      <c r="J22" s="43"/>
-      <c r="K22" s="33"/>
-      <c r="L22" s="34"/>
-      <c r="M22" s="40"/>
+      <c r="B22" s="35"/>
+      <c r="C22" s="34"/>
+      <c r="D22" s="34"/>
+      <c r="E22" s="34"/>
+      <c r="F22" s="34"/>
+      <c r="G22" s="34"/>
+      <c r="H22" s="34"/>
+      <c r="I22" s="34"/>
+      <c r="J22" s="36"/>
+      <c r="K22" s="109"/>
+      <c r="L22" s="113"/>
+      <c r="M22" s="33"/>
     </row>
     <row r="23" spans="1:16" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="15"/>
-      <c r="B23" s="42"/>
-      <c r="C23" s="41"/>
-      <c r="D23" s="41"/>
-      <c r="E23" s="41"/>
-      <c r="F23" s="41"/>
-      <c r="G23" s="41"/>
-      <c r="H23" s="41"/>
-      <c r="I23" s="41"/>
-      <c r="J23" s="41"/>
-      <c r="K23" s="37"/>
-      <c r="L23" s="38"/>
+      <c r="B23" s="35"/>
+      <c r="C23" s="34"/>
+      <c r="D23" s="34"/>
+      <c r="E23" s="34"/>
+      <c r="F23" s="34"/>
+      <c r="G23" s="34"/>
+      <c r="H23" s="34"/>
+      <c r="I23" s="34"/>
+      <c r="J23" s="34"/>
+      <c r="K23" s="110"/>
+      <c r="L23" s="114"/>
       <c r="M23" s="17"/>
     </row>
     <row r="24" spans="1:16" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="15"/>
-      <c r="B24" s="42"/>
-      <c r="C24" s="41"/>
-      <c r="D24" s="41"/>
-      <c r="E24" s="41"/>
-      <c r="F24" s="41"/>
-      <c r="G24" s="41"/>
-      <c r="H24" s="41"/>
-      <c r="I24" s="41"/>
-      <c r="J24" s="41"/>
-      <c r="K24" s="35"/>
-      <c r="L24" s="36"/>
+      <c r="B24" s="35"/>
+      <c r="C24" s="34"/>
+      <c r="D24" s="34"/>
+      <c r="E24" s="34"/>
+      <c r="F24" s="34"/>
+      <c r="G24" s="34"/>
+      <c r="H24" s="34"/>
+      <c r="I24" s="34"/>
+      <c r="J24" s="34"/>
+      <c r="K24" s="111"/>
+      <c r="L24" s="115"/>
       <c r="M24" s="18"/>
     </row>
     <row r="25" spans="1:16" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="44"/>
-      <c r="C25" s="45"/>
-      <c r="D25" s="45"/>
-      <c r="E25" s="45"/>
-      <c r="F25" s="45"/>
-      <c r="G25" s="45"/>
-      <c r="H25" s="45"/>
-      <c r="I25" s="45"/>
-      <c r="J25" s="45"/>
-      <c r="K25" s="37"/>
-      <c r="L25" s="38"/>
-      <c r="M25" s="81"/>
+      <c r="B25" s="37"/>
+      <c r="C25" s="38"/>
+      <c r="D25" s="38"/>
+      <c r="E25" s="38"/>
+      <c r="F25" s="38"/>
+      <c r="G25" s="38"/>
+      <c r="H25" s="38"/>
+      <c r="I25" s="38"/>
+      <c r="J25" s="38"/>
+      <c r="K25" s="110"/>
+      <c r="L25" s="114"/>
+      <c r="M25" s="73"/>
     </row>
     <row r="26" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="46"/>
-      <c r="C26" s="47"/>
+      <c r="B26" s="39"/>
+      <c r="C26" s="40"/>
       <c r="D26" s="31"/>
       <c r="E26" s="31"/>
       <c r="F26" s="31"/>
       <c r="G26" s="31"/>
       <c r="H26" s="31"/>
-      <c r="I26" s="48"/>
-      <c r="J26" s="48"/>
-      <c r="K26" s="37"/>
-      <c r="L26" s="38"/>
+      <c r="I26" s="41"/>
+      <c r="J26" s="41"/>
+      <c r="K26" s="110"/>
+      <c r="L26" s="114"/>
       <c r="M26" s="17"/>
     </row>
     <row r="27" spans="1:16" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="44"/>
-      <c r="C27" s="48"/>
-      <c r="D27" s="48"/>
-      <c r="E27" s="48"/>
-      <c r="F27" s="48"/>
-      <c r="G27" s="48"/>
-      <c r="H27" s="48"/>
-      <c r="I27" s="48"/>
-      <c r="J27" s="48"/>
-      <c r="K27" s="37"/>
-      <c r="L27" s="38"/>
+      <c r="B27" s="37"/>
+      <c r="C27" s="41"/>
+      <c r="D27" s="41"/>
+      <c r="E27" s="41"/>
+      <c r="F27" s="41"/>
+      <c r="G27" s="41"/>
+      <c r="H27" s="41"/>
+      <c r="I27" s="41"/>
+      <c r="J27" s="41"/>
+      <c r="K27" s="110"/>
+      <c r="L27" s="114"/>
       <c r="M27" s="17"/>
     </row>
     <row r="28" spans="1:16" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="49"/>
-      <c r="C28" s="50"/>
-      <c r="D28" s="50"/>
-      <c r="E28" s="50"/>
-      <c r="F28" s="50"/>
-      <c r="G28" s="50"/>
-      <c r="H28" s="50"/>
-      <c r="I28" s="50"/>
-      <c r="J28" s="50"/>
-      <c r="K28" s="39"/>
-      <c r="L28" s="74"/>
+      <c r="B28" s="42"/>
+      <c r="C28" s="43"/>
+      <c r="D28" s="43"/>
+      <c r="E28" s="43"/>
+      <c r="F28" s="43"/>
+      <c r="G28" s="43"/>
+      <c r="H28" s="43"/>
+      <c r="I28" s="43"/>
+      <c r="J28" s="43"/>
+      <c r="K28" s="112"/>
+      <c r="L28" s="116"/>
       <c r="M28" s="17"/>
     </row>
     <row r="29" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
@@ -1684,8 +1682,8 @@
       <c r="K29" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="L29" s="86"/>
-      <c r="M29" s="71"/>
+      <c r="L29" s="78"/>
+      <c r="M29" s="64"/>
     </row>
     <row r="30" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="19"/>
@@ -1700,28 +1698,28 @@
       <c r="K30" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="L30" s="86"/>
-      <c r="M30" s="71"/>
+      <c r="L30" s="78"/>
+      <c r="M30" s="64"/>
     </row>
     <row r="31" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="112"/>
-      <c r="C31" s="113"/>
-      <c r="D31" s="113"/>
-      <c r="E31" s="113"/>
-      <c r="F31" s="113"/>
-      <c r="G31" s="113"/>
-      <c r="H31" s="113"/>
-      <c r="I31" s="113"/>
-      <c r="J31" s="114"/>
-      <c r="K31" s="104" t="s">
+      <c r="B31" s="80"/>
+      <c r="C31" s="81"/>
+      <c r="D31" s="81"/>
+      <c r="E31" s="81"/>
+      <c r="F31" s="81"/>
+      <c r="G31" s="81"/>
+      <c r="H31" s="81"/>
+      <c r="I31" s="81"/>
+      <c r="J31" s="82"/>
+      <c r="K31" s="93" t="s">
         <v>28</v>
       </c>
-      <c r="L31" s="56"/>
-      <c r="M31" s="72"/>
+      <c r="L31" s="49"/>
+      <c r="M31" s="65"/>
     </row>
     <row r="32" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="15"/>
-      <c r="B32" s="115"/>
+      <c r="B32" s="83"/>
       <c r="C32" s="30"/>
       <c r="D32" s="30"/>
       <c r="E32" s="30"/>
@@ -1729,86 +1727,86 @@
       <c r="G32" s="30"/>
       <c r="H32" s="30"/>
       <c r="I32" s="30"/>
-      <c r="J32" s="116"/>
-      <c r="K32" s="105"/>
+      <c r="J32" s="84"/>
+      <c r="K32" s="94"/>
       <c r="L32" s="24"/>
-      <c r="M32" s="73"/>
+      <c r="M32" s="66"/>
       <c r="P32" s="14"/>
     </row>
     <row r="33" spans="2:16" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="52"/>
-      <c r="C33" s="53"/>
-      <c r="D33" s="53"/>
-      <c r="E33" s="53"/>
-      <c r="F33" s="53"/>
-      <c r="G33" s="53"/>
-      <c r="H33" s="53"/>
-      <c r="I33" s="53"/>
-      <c r="J33" s="54"/>
+      <c r="B33" s="45"/>
+      <c r="C33" s="46"/>
+      <c r="D33" s="46"/>
+      <c r="E33" s="46"/>
+      <c r="F33" s="46"/>
+      <c r="G33" s="46"/>
+      <c r="H33" s="46"/>
+      <c r="I33" s="46"/>
+      <c r="J33" s="47"/>
       <c r="K33" s="21" t="s">
         <v>9</v>
       </c>
       <c r="L33" s="22"/>
-      <c r="M33" s="75">
+      <c r="M33" s="67">
         <f>SUM(M29:M32)</f>
         <v>0</v>
       </c>
       <c r="P33" s="13"/>
     </row>
     <row r="34" spans="2:16" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B34" s="55"/>
-      <c r="C34" s="51"/>
-      <c r="D34" s="51"/>
-      <c r="E34" s="51"/>
-      <c r="F34" s="51"/>
-      <c r="G34" s="51"/>
-      <c r="H34" s="51"/>
-      <c r="I34" s="51"/>
-      <c r="J34" s="51"/>
-      <c r="K34" s="78" t="s">
+      <c r="B34" s="48"/>
+      <c r="C34" s="44"/>
+      <c r="D34" s="44"/>
+      <c r="E34" s="44"/>
+      <c r="F34" s="44"/>
+      <c r="G34" s="44"/>
+      <c r="H34" s="44"/>
+      <c r="I34" s="44"/>
+      <c r="J34" s="44"/>
+      <c r="K34" s="70" t="s">
         <v>8</v>
       </c>
       <c r="L34" s="22"/>
-      <c r="M34" s="76"/>
-      <c r="O34" s="106"/>
-      <c r="P34" s="98"/>
+      <c r="M34" s="68"/>
+      <c r="O34" s="95"/>
+      <c r="P34" s="87"/>
     </row>
     <row r="35" spans="2:16" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B35" s="99" t="s">
+      <c r="B35" s="88" t="s">
         <v>7</v>
       </c>
-      <c r="C35" s="100"/>
-      <c r="D35" s="100"/>
-      <c r="E35" s="100"/>
-      <c r="F35" s="100"/>
-      <c r="G35" s="100"/>
-      <c r="H35" s="100"/>
-      <c r="I35" s="100"/>
-      <c r="J35" s="100"/>
-      <c r="K35" s="79"/>
-      <c r="L35" s="87"/>
-      <c r="M35" s="77"/>
-      <c r="O35" s="106"/>
-      <c r="P35" s="98"/>
+      <c r="C35" s="89"/>
+      <c r="D35" s="89"/>
+      <c r="E35" s="89"/>
+      <c r="F35" s="89"/>
+      <c r="G35" s="89"/>
+      <c r="H35" s="89"/>
+      <c r="I35" s="89"/>
+      <c r="J35" s="89"/>
+      <c r="K35" s="71"/>
+      <c r="L35" s="79"/>
+      <c r="M35" s="69"/>
+      <c r="O35" s="95"/>
+      <c r="P35" s="87"/>
     </row>
     <row r="36" spans="2:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B36" s="101"/>
-      <c r="C36" s="102"/>
-      <c r="D36" s="102"/>
-      <c r="E36" s="102"/>
-      <c r="F36" s="102"/>
-      <c r="G36" s="102"/>
-      <c r="H36" s="102"/>
-      <c r="I36" s="102"/>
-      <c r="J36" s="103"/>
+      <c r="B36" s="90"/>
+      <c r="C36" s="91"/>
+      <c r="D36" s="91"/>
+      <c r="E36" s="91"/>
+      <c r="F36" s="91"/>
+      <c r="G36" s="91"/>
+      <c r="H36" s="91"/>
+      <c r="I36" s="91"/>
+      <c r="J36" s="92"/>
       <c r="K36" s="6" t="s">
         <v>6</v>
       </c>
       <c r="L36" s="23"/>
-      <c r="M36" s="73"/>
+      <c r="M36" s="66"/>
     </row>
     <row r="37" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B37" s="70" t="s">
+      <c r="B37" s="63" t="s">
         <v>5</v>
       </c>
       <c r="C37" s="5"/>
@@ -1818,7 +1816,7 @@
       <c r="G37" s="5"/>
       <c r="H37" s="5"/>
       <c r="I37" s="5"/>
-      <c r="J37" s="69"/>
+      <c r="J37" s="62"/>
       <c r="K37" s="4"/>
       <c r="L37" s="4"/>
       <c r="M37" s="4"/>
@@ -1894,24 +1892,24 @@
       <c r="M42" s="5"/>
     </row>
     <row r="43" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B43" s="108" t="s">
+      <c r="B43" s="105" t="s">
         <v>4</v>
       </c>
-      <c r="C43" s="108"/>
-      <c r="D43" s="108"/>
-      <c r="E43" s="108"/>
-      <c r="F43" s="108"/>
+      <c r="C43" s="105"/>
+      <c r="D43" s="105"/>
+      <c r="E43" s="105"/>
+      <c r="F43" s="105"/>
       <c r="G43" s="4"/>
-      <c r="H43" s="109" t="s">
+      <c r="H43" s="106" t="s">
         <v>3</v>
       </c>
-      <c r="I43" s="109"/>
-      <c r="J43" s="109"/>
+      <c r="I43" s="106"/>
+      <c r="J43" s="106"/>
       <c r="K43" s="3"/>
-      <c r="L43" s="110" t="s">
+      <c r="L43" s="107" t="s">
         <v>2</v>
       </c>
-      <c r="M43" s="110"/>
+      <c r="M43" s="107"/>
       <c r="N43" s="12"/>
       <c r="O43" s="12"/>
       <c r="P43" s="12"/>
@@ -1923,74 +1921,74 @@
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
       <c r="G44" s="2"/>
-      <c r="H44" s="109"/>
-      <c r="I44" s="109"/>
-      <c r="J44" s="109"/>
+      <c r="H44" s="106"/>
+      <c r="I44" s="106"/>
+      <c r="J44" s="106"/>
       <c r="K44" s="1"/>
       <c r="L44" s="1"/>
       <c r="M44" s="1"/>
     </row>
     <row r="45" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B45" s="111"/>
-      <c r="C45" s="111"/>
-      <c r="D45" s="111"/>
-      <c r="E45" s="111"/>
-      <c r="F45" s="111"/>
-      <c r="G45" s="111"/>
-      <c r="H45" s="111"/>
-      <c r="I45" s="111"/>
-      <c r="J45" s="111"/>
-      <c r="K45" s="111"/>
-      <c r="L45" s="111"/>
-      <c r="M45" s="111"/>
+      <c r="B45" s="108"/>
+      <c r="C45" s="108"/>
+      <c r="D45" s="108"/>
+      <c r="E45" s="108"/>
+      <c r="F45" s="108"/>
+      <c r="G45" s="108"/>
+      <c r="H45" s="108"/>
+      <c r="I45" s="108"/>
+      <c r="J45" s="108"/>
+      <c r="K45" s="108"/>
+      <c r="L45" s="108"/>
+      <c r="M45" s="108"/>
     </row>
     <row r="46" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B46" s="107" t="s">
+      <c r="B46" s="104" t="s">
         <v>27</v>
       </c>
-      <c r="C46" s="107"/>
-      <c r="D46" s="107"/>
-      <c r="E46" s="107"/>
-      <c r="F46" s="107"/>
-      <c r="G46" s="107"/>
-      <c r="H46" s="107"/>
-      <c r="I46" s="107"/>
-      <c r="J46" s="107"/>
-      <c r="K46" s="107"/>
-      <c r="L46" s="107"/>
-      <c r="M46" s="107"/>
+      <c r="C46" s="104"/>
+      <c r="D46" s="104"/>
+      <c r="E46" s="104"/>
+      <c r="F46" s="104"/>
+      <c r="G46" s="104"/>
+      <c r="H46" s="104"/>
+      <c r="I46" s="104"/>
+      <c r="J46" s="104"/>
+      <c r="K46" s="104"/>
+      <c r="L46" s="104"/>
+      <c r="M46" s="104"/>
     </row>
     <row r="47" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B47" s="107" t="s">
+      <c r="B47" s="104" t="s">
         <v>1</v>
       </c>
-      <c r="C47" s="107"/>
-      <c r="D47" s="107"/>
-      <c r="E47" s="107"/>
-      <c r="F47" s="107"/>
-      <c r="G47" s="107"/>
-      <c r="H47" s="107"/>
-      <c r="I47" s="107"/>
-      <c r="J47" s="107"/>
-      <c r="K47" s="107"/>
-      <c r="L47" s="107"/>
-      <c r="M47" s="107"/>
+      <c r="C47" s="104"/>
+      <c r="D47" s="104"/>
+      <c r="E47" s="104"/>
+      <c r="F47" s="104"/>
+      <c r="G47" s="104"/>
+      <c r="H47" s="104"/>
+      <c r="I47" s="104"/>
+      <c r="J47" s="104"/>
+      <c r="K47" s="104"/>
+      <c r="L47" s="104"/>
+      <c r="M47" s="104"/>
     </row>
     <row r="48" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B48" s="107" t="s">
+      <c r="B48" s="104" t="s">
         <v>0</v>
       </c>
-      <c r="C48" s="107"/>
-      <c r="D48" s="107"/>
-      <c r="E48" s="107"/>
-      <c r="F48" s="107"/>
-      <c r="G48" s="107"/>
-      <c r="H48" s="107"/>
-      <c r="I48" s="107"/>
-      <c r="J48" s="107"/>
-      <c r="K48" s="107"/>
-      <c r="L48" s="107"/>
-      <c r="M48" s="107"/>
+      <c r="C48" s="104"/>
+      <c r="D48" s="104"/>
+      <c r="E48" s="104"/>
+      <c r="F48" s="104"/>
+      <c r="G48" s="104"/>
+      <c r="H48" s="104"/>
+      <c r="I48" s="104"/>
+      <c r="J48" s="104"/>
+      <c r="K48" s="104"/>
+      <c r="L48" s="104"/>
+      <c r="M48" s="104"/>
     </row>
   </sheetData>
   <mergeCells count="18">

</xml_diff>

<commit_message>
correccion edicion entidades usuario3
</commit_message>
<xml_diff>
--- a/storage/plantillas_excel/Schlumberger Surenco.xlsx
+++ b/storage/plantillas_excel/Schlumberger Surenco.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Bogota D.C. - Colombia</t>
   </si>
@@ -50,9 +50,6 @@
     <t xml:space="preserve">Impreso en computador por   SYSTEM INTEGRAL GROUP S.A.S.     Nit 800.089.229 - 4    Calle 154 No. 19A - 20. </t>
   </si>
   <si>
-    <t>$</t>
-  </si>
-  <si>
     <t>TOTAL</t>
   </si>
   <si>
@@ -68,41 +65,7 @@
     <t>SUBTOTAL</t>
   </si>
   <si>
-    <t xml:space="preserve">SON:  </t>
-  </si>
-  <si>
     <t>REEMBOLSO DE   GASTOS    NO GENERADORES DE IVA</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">CONSIGNAR A NOMBRE DE SYSTEM INTEGRAL GROUP S.A.S.  </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">BANCO BBVA CUENTA DE AHORROS </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>479271454</t>
-    </r>
   </si>
   <si>
     <t>INGRESOS EXCLUIDOS DE IVA</t>
@@ -178,12 +141,12 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="7">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;\ #,##0"/>
-    <numFmt numFmtId="165" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="166" formatCode="_ &quot;$&quot;\ * #,##0.00_ ;_ &quot;$&quot;\ * \-#,##0.00_ ;_ &quot;$&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="167" formatCode="&quot;$&quot;\ #,##0;&quot;$&quot;\ \-#,##0"/>
     <numFmt numFmtId="168" formatCode="&quot;$&quot;\ #,##0.00;&quot;$&quot;\ \-#,##0.00"/>
     <numFmt numFmtId="169" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="170" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="173" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
   <fonts count="13" x14ac:knownFonts="1">
     <font>
@@ -279,7 +242,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -443,6 +406,19 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -450,7 +426,7 @@
     <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="169" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="111">
+  <cellXfs count="117">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -461,15 +437,11 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -498,16 +470,8 @@
     <xf numFmtId="164" fontId="9" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="distributed" wrapText="1"/>
     </xf>
@@ -521,27 +485,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="distributed" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="distributed" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="distributed" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="distributed" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="distributed" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="distributed" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -571,9 +522,6 @@
     <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="15" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -603,53 +551,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="1" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="170" fontId="1" fillId="3" borderId="14" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="170" fontId="1" fillId="3" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="distributed" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="distributed" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="1" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="168" fontId="1" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="distributed" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="1" fillId="3" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="167" fontId="1" fillId="3" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -703,33 +604,12 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="justify"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="justify"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="justify"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="justify"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="justify"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="justify"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -741,6 +621,124 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="justify"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="justify"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="justify"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="justify"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="justify"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="justify"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="1" fillId="3" borderId="14" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="1" fillId="3" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="1" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="1" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="1" fillId="3" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="1" fillId="3" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="1" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="1" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="173" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1214,8 +1212,8 @@
   </sheetPr>
   <dimension ref="A1:P47"/>
   <sheetViews>
-    <sheetView showGridLines="0" showZeros="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17:J18"/>
+    <sheetView showGridLines="0" showZeros="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A25" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1262,8 +1260,8 @@
       <c r="J2" s="6"/>
       <c r="K2" s="6"/>
       <c r="L2" s="6"/>
-      <c r="M2" s="49" t="s">
-        <v>36</v>
+      <c r="M2" s="38" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="2:13" ht="6" customHeight="1" x14ac:dyDescent="0.2">
@@ -1290,44 +1288,44 @@
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
-      <c r="K4" s="48"/>
-      <c r="L4" s="48"/>
-      <c r="M4" s="47" t="s">
-        <v>35</v>
+      <c r="K4" s="37"/>
+      <c r="L4" s="37"/>
+      <c r="M4" s="36" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="2:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="50"/>
-      <c r="C5" s="50"/>
-      <c r="D5" s="50"/>
-      <c r="E5" s="50"/>
-      <c r="F5" s="50"/>
-      <c r="G5" s="50"/>
-      <c r="H5" s="50"/>
-      <c r="I5" s="50"/>
-      <c r="J5" s="50"/>
-      <c r="K5" s="48"/>
-      <c r="L5" s="48"/>
-      <c r="M5" s="47" t="s">
-        <v>34</v>
+      <c r="B5" s="39"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="39"/>
+      <c r="F5" s="39"/>
+      <c r="G5" s="39"/>
+      <c r="H5" s="39"/>
+      <c r="I5" s="39"/>
+      <c r="J5" s="39"/>
+      <c r="K5" s="37"/>
+      <c r="L5" s="37"/>
+      <c r="M5" s="36" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B6" s="51" t="s">
-        <v>33</v>
-      </c>
-      <c r="C6" s="51"/>
-      <c r="D6" s="51"/>
-      <c r="E6" s="51"/>
-      <c r="F6" s="51"/>
-      <c r="G6" s="51"/>
-      <c r="H6" s="51"/>
-      <c r="I6" s="51"/>
-      <c r="J6" s="51"/>
-      <c r="K6" s="48"/>
-      <c r="L6" s="48"/>
-      <c r="M6" s="47" t="s">
-        <v>32</v>
+      <c r="B6" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="40"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="40"/>
+      <c r="I6" s="40"/>
+      <c r="J6" s="40"/>
+      <c r="K6" s="37"/>
+      <c r="L6" s="37"/>
+      <c r="M6" s="36" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.2">
@@ -1340,10 +1338,10 @@
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
-      <c r="K7" s="48"/>
-      <c r="L7" s="48"/>
-      <c r="M7" s="47" t="s">
-        <v>31</v>
+      <c r="K7" s="37"/>
+      <c r="L7" s="37"/>
+      <c r="M7" s="36" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.2">
@@ -1356,10 +1354,10 @@
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
-      <c r="K8" s="48"/>
-      <c r="L8" s="48"/>
-      <c r="M8" s="47" t="s">
-        <v>30</v>
+      <c r="K8" s="37"/>
+      <c r="L8" s="37"/>
+      <c r="M8" s="36" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.2">
@@ -1374,83 +1372,83 @@
       <c r="J9" s="6"/>
       <c r="K9" s="6"/>
       <c r="L9" s="6"/>
-      <c r="M9" s="46" t="s">
-        <v>29</v>
+      <c r="M9" s="35" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="2:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" s="52"/>
-      <c r="D10" s="52"/>
-      <c r="E10" s="52"/>
-      <c r="F10" s="52"/>
+        <v>25</v>
+      </c>
+      <c r="C10" s="75"/>
+      <c r="D10" s="75"/>
+      <c r="E10" s="75"/>
+      <c r="F10" s="75"/>
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
-      <c r="I10" s="53" t="s">
-        <v>27</v>
-      </c>
-      <c r="J10" s="53"/>
-      <c r="K10" s="45"/>
+      <c r="I10" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="J10" s="41"/>
+      <c r="K10" s="34"/>
       <c r="L10" s="6"/>
-      <c r="M10" s="54" t="s">
-        <v>26</v>
+      <c r="M10" s="42" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="2:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="56" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="56"/>
-      <c r="D11" s="56"/>
-      <c r="E11" s="57"/>
-      <c r="F11" s="57"/>
-      <c r="G11" s="57"/>
-      <c r="H11" s="57"/>
-      <c r="I11" s="57"/>
-      <c r="J11" s="57"/>
-      <c r="K11" s="57"/>
+      <c r="B11" s="44" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="44"/>
+      <c r="D11" s="44"/>
+      <c r="E11" s="45"/>
+      <c r="F11" s="45"/>
+      <c r="G11" s="45"/>
+      <c r="H11" s="45"/>
+      <c r="I11" s="45"/>
+      <c r="J11" s="45"/>
+      <c r="K11" s="45"/>
       <c r="L11" s="6"/>
-      <c r="M11" s="55"/>
+      <c r="M11" s="43"/>
     </row>
     <row r="12" spans="2:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" s="58"/>
-      <c r="D12" s="58"/>
-      <c r="E12" s="58"/>
-      <c r="F12" s="58"/>
-      <c r="G12" s="58"/>
-      <c r="H12" s="58"/>
-      <c r="I12" s="58"/>
-      <c r="J12" s="44" t="s">
-        <v>23</v>
-      </c>
-      <c r="K12" s="43"/>
+        <v>21</v>
+      </c>
+      <c r="C12" s="46"/>
+      <c r="D12" s="46"/>
+      <c r="E12" s="46"/>
+      <c r="F12" s="46"/>
+      <c r="G12" s="46"/>
+      <c r="H12" s="46"/>
+      <c r="I12" s="46"/>
+      <c r="J12" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="K12" s="32"/>
       <c r="L12" s="6"/>
-      <c r="M12" s="59" t="s">
-        <v>37</v>
+      <c r="M12" s="47" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="2:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="60" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" s="60"/>
-      <c r="D13" s="61"/>
-      <c r="E13" s="61"/>
-      <c r="F13" s="61"/>
-      <c r="G13" s="61"/>
-      <c r="H13" s="61"/>
-      <c r="I13" s="61"/>
-      <c r="J13" s="44" t="s">
-        <v>21</v>
-      </c>
-      <c r="K13" s="43"/>
+      <c r="B13" s="48" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="48"/>
+      <c r="D13" s="49"/>
+      <c r="E13" s="49"/>
+      <c r="F13" s="49"/>
+      <c r="G13" s="49"/>
+      <c r="H13" s="49"/>
+      <c r="I13" s="49"/>
+      <c r="J13" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="K13" s="32"/>
       <c r="L13" s="6"/>
-      <c r="M13" s="59"/>
+      <c r="M13" s="47"/>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B14" s="6"/>
@@ -1481,412 +1479,387 @@
       <c r="M15" s="6"/>
     </row>
     <row r="16" spans="2:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="62" t="s">
-        <v>20</v>
-      </c>
-      <c r="C16" s="62"/>
-      <c r="D16" s="62"/>
-      <c r="E16" s="62"/>
-      <c r="F16" s="62"/>
-      <c r="G16" s="62"/>
-      <c r="H16" s="62"/>
-      <c r="I16" s="62"/>
-      <c r="J16" s="62"/>
-      <c r="K16" s="62" t="s">
-        <v>19</v>
-      </c>
-      <c r="L16" s="62"/>
-      <c r="M16" s="42" t="s">
-        <v>18</v>
+      <c r="B16" s="50" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="50"/>
+      <c r="D16" s="50"/>
+      <c r="E16" s="50"/>
+      <c r="F16" s="50"/>
+      <c r="G16" s="50"/>
+      <c r="H16" s="50"/>
+      <c r="I16" s="50"/>
+      <c r="J16" s="50"/>
+      <c r="K16" s="50" t="s">
+        <v>16</v>
+      </c>
+      <c r="L16" s="109"/>
+      <c r="M16" s="31" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:13" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="18"/>
-      <c r="B17" s="63"/>
-      <c r="C17" s="64"/>
-      <c r="D17" s="64"/>
-      <c r="E17" s="64"/>
-      <c r="F17" s="64"/>
-      <c r="G17" s="64"/>
-      <c r="H17" s="64"/>
-      <c r="I17" s="64"/>
-      <c r="J17" s="65"/>
-      <c r="K17" s="66"/>
-      <c r="L17" s="66"/>
-      <c r="M17" s="28"/>
+      <c r="A17" s="16"/>
+      <c r="B17" s="82"/>
+      <c r="C17" s="83"/>
+      <c r="D17" s="83"/>
+      <c r="E17" s="83"/>
+      <c r="F17" s="83"/>
+      <c r="G17" s="83"/>
+      <c r="H17" s="83"/>
+      <c r="I17" s="83"/>
+      <c r="J17" s="84"/>
+      <c r="K17" s="108"/>
+      <c r="L17" s="111"/>
+      <c r="M17" s="113"/>
     </row>
     <row r="18" spans="1:13" ht="81" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="18"/>
-      <c r="B18" s="63"/>
-      <c r="C18" s="64"/>
-      <c r="D18" s="64"/>
-      <c r="E18" s="64"/>
-      <c r="F18" s="64"/>
-      <c r="G18" s="64"/>
-      <c r="H18" s="64"/>
-      <c r="I18" s="64"/>
-      <c r="J18" s="65"/>
-      <c r="K18" s="67"/>
-      <c r="L18" s="68"/>
-      <c r="M18" s="41"/>
+      <c r="A18" s="16"/>
+      <c r="B18" s="82"/>
+      <c r="C18" s="83"/>
+      <c r="D18" s="83"/>
+      <c r="E18" s="83"/>
+      <c r="F18" s="83"/>
+      <c r="G18" s="83"/>
+      <c r="H18" s="83"/>
+      <c r="I18" s="83"/>
+      <c r="J18" s="84"/>
+      <c r="K18" s="102"/>
+      <c r="L18" s="103"/>
+      <c r="M18" s="113"/>
     </row>
     <row r="19" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="18"/>
-      <c r="B19" s="31"/>
-      <c r="C19" s="69"/>
-      <c r="D19" s="69"/>
-      <c r="E19" s="69"/>
-      <c r="F19" s="69"/>
-      <c r="G19" s="69"/>
-      <c r="H19" s="69"/>
-      <c r="I19" s="69"/>
-      <c r="J19" s="70"/>
-      <c r="K19" s="66"/>
-      <c r="L19" s="66"/>
-      <c r="M19" s="28"/>
+      <c r="A19" s="16"/>
+      <c r="B19" s="85"/>
+      <c r="C19" s="83"/>
+      <c r="D19" s="83"/>
+      <c r="E19" s="83"/>
+      <c r="F19" s="83"/>
+      <c r="G19" s="83"/>
+      <c r="H19" s="83"/>
+      <c r="I19" s="83"/>
+      <c r="J19" s="84"/>
+      <c r="K19" s="104"/>
+      <c r="L19" s="105"/>
+      <c r="M19" s="112"/>
     </row>
     <row r="20" spans="1:13" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="18"/>
-      <c r="B20" s="40"/>
-      <c r="C20" s="69"/>
-      <c r="D20" s="71"/>
-      <c r="E20" s="71"/>
-      <c r="F20" s="71"/>
-      <c r="G20" s="71"/>
-      <c r="H20" s="71"/>
-      <c r="I20" s="71"/>
-      <c r="J20" s="72"/>
-      <c r="K20" s="66"/>
-      <c r="L20" s="66"/>
-      <c r="M20" s="28"/>
+      <c r="A20" s="16"/>
+      <c r="B20" s="86"/>
+      <c r="C20" s="83"/>
+      <c r="D20" s="87"/>
+      <c r="E20" s="87"/>
+      <c r="F20" s="87"/>
+      <c r="G20" s="87"/>
+      <c r="H20" s="87"/>
+      <c r="I20" s="87"/>
+      <c r="J20" s="88"/>
+      <c r="K20" s="104"/>
+      <c r="L20" s="105"/>
+      <c r="M20" s="113"/>
     </row>
     <row r="21" spans="1:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="18"/>
-      <c r="B21" s="40"/>
-      <c r="C21" s="64"/>
-      <c r="D21" s="64"/>
-      <c r="E21" s="64"/>
-      <c r="F21" s="64"/>
-      <c r="G21" s="64"/>
-      <c r="H21" s="64"/>
-      <c r="I21" s="64"/>
-      <c r="J21" s="65"/>
-      <c r="K21" s="66"/>
-      <c r="L21" s="66"/>
-      <c r="M21" s="28"/>
+      <c r="A21" s="16"/>
+      <c r="B21" s="82"/>
+      <c r="C21" s="83"/>
+      <c r="D21" s="83"/>
+      <c r="E21" s="83"/>
+      <c r="F21" s="83"/>
+      <c r="G21" s="83"/>
+      <c r="H21" s="83"/>
+      <c r="I21" s="83"/>
+      <c r="J21" s="84"/>
+      <c r="K21" s="104"/>
+      <c r="L21" s="105"/>
+      <c r="M21" s="112"/>
     </row>
     <row r="22" spans="1:13" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="18"/>
-      <c r="B22" s="39"/>
-      <c r="C22" s="64"/>
-      <c r="D22" s="64"/>
-      <c r="E22" s="64"/>
-      <c r="F22" s="64"/>
-      <c r="G22" s="64"/>
-      <c r="H22" s="64"/>
-      <c r="I22" s="64"/>
-      <c r="J22" s="65"/>
-      <c r="K22" s="66"/>
-      <c r="L22" s="66"/>
-      <c r="M22" s="28"/>
+      <c r="A22" s="16"/>
+      <c r="B22" s="82"/>
+      <c r="C22" s="83"/>
+      <c r="D22" s="83"/>
+      <c r="E22" s="83"/>
+      <c r="F22" s="83"/>
+      <c r="G22" s="83"/>
+      <c r="H22" s="83"/>
+      <c r="I22" s="83"/>
+      <c r="J22" s="84"/>
+      <c r="K22" s="104"/>
+      <c r="L22" s="105"/>
+      <c r="M22" s="112"/>
     </row>
     <row r="23" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="18"/>
-      <c r="B23" s="31"/>
-      <c r="C23" s="73"/>
-      <c r="D23" s="73"/>
-      <c r="E23" s="73"/>
-      <c r="F23" s="73"/>
-      <c r="G23" s="73"/>
-      <c r="H23" s="73"/>
-      <c r="I23" s="73"/>
-      <c r="J23" s="74"/>
-      <c r="K23" s="66"/>
-      <c r="L23" s="66"/>
-      <c r="M23" s="28"/>
+      <c r="A23" s="16"/>
+      <c r="B23" s="85"/>
+      <c r="C23" s="89"/>
+      <c r="D23" s="89"/>
+      <c r="E23" s="89"/>
+      <c r="F23" s="89"/>
+      <c r="G23" s="89"/>
+      <c r="H23" s="89"/>
+      <c r="I23" s="89"/>
+      <c r="J23" s="90"/>
+      <c r="K23" s="104"/>
+      <c r="L23" s="105"/>
+      <c r="M23" s="113"/>
     </row>
     <row r="24" spans="1:13" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="31"/>
-      <c r="C24" s="69"/>
-      <c r="D24" s="71"/>
-      <c r="E24" s="71"/>
-      <c r="F24" s="71"/>
-      <c r="G24" s="71"/>
-      <c r="H24" s="71"/>
-      <c r="I24" s="71"/>
-      <c r="J24" s="72"/>
-      <c r="K24" s="66"/>
-      <c r="L24" s="66"/>
-      <c r="M24" s="28"/>
+      <c r="B24" s="25"/>
+      <c r="C24" s="27"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="26"/>
+      <c r="G24" s="26"/>
+      <c r="H24" s="26"/>
+      <c r="I24" s="26"/>
+      <c r="J24" s="92"/>
+      <c r="K24" s="104"/>
+      <c r="L24" s="105"/>
+      <c r="M24" s="112"/>
     </row>
     <row r="25" spans="1:13" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="38"/>
-      <c r="C25" s="69"/>
-      <c r="D25" s="71"/>
-      <c r="E25" s="71"/>
-      <c r="F25" s="71"/>
-      <c r="G25" s="71"/>
-      <c r="H25" s="71"/>
-      <c r="I25" s="71"/>
-      <c r="J25" s="72"/>
-      <c r="K25" s="66"/>
-      <c r="L25" s="66"/>
-      <c r="M25" s="28"/>
+      <c r="B25" s="91"/>
+      <c r="C25" s="83"/>
+      <c r="D25" s="87"/>
+      <c r="E25" s="87"/>
+      <c r="F25" s="87"/>
+      <c r="G25" s="87"/>
+      <c r="H25" s="87"/>
+      <c r="I25" s="87"/>
+      <c r="J25" s="88"/>
+      <c r="K25" s="104"/>
+      <c r="L25" s="105"/>
+      <c r="M25" s="113"/>
     </row>
     <row r="26" spans="1:13" ht="5.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="37"/>
-      <c r="C26" s="36"/>
-      <c r="D26" s="36"/>
-      <c r="E26" s="36"/>
-      <c r="F26" s="36"/>
-      <c r="G26" s="36"/>
-      <c r="H26" s="36"/>
-      <c r="I26" s="36"/>
-      <c r="J26" s="35"/>
-      <c r="K26" s="66"/>
-      <c r="L26" s="66"/>
-      <c r="M26" s="28">
-        <f>+K26*E26</f>
-        <v>0</v>
-      </c>
+      <c r="B26" s="29"/>
+      <c r="C26" s="28"/>
+      <c r="D26" s="28"/>
+      <c r="E26" s="28"/>
+      <c r="F26" s="28"/>
+      <c r="G26" s="28"/>
+      <c r="H26" s="28"/>
+      <c r="I26" s="28"/>
+      <c r="J26" s="101"/>
+      <c r="K26" s="104"/>
+      <c r="L26" s="105"/>
+      <c r="M26" s="112"/>
     </row>
     <row r="27" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="34"/>
-      <c r="C27" s="33"/>
-      <c r="D27" s="32"/>
-      <c r="E27" s="32"/>
-      <c r="F27" s="32"/>
-      <c r="G27" s="32"/>
-      <c r="H27" s="32"/>
-      <c r="I27" s="30"/>
-      <c r="J27" s="29"/>
-      <c r="K27" s="75"/>
-      <c r="L27" s="76"/>
-      <c r="M27" s="28"/>
+      <c r="B27" s="93"/>
+      <c r="C27" s="27"/>
+      <c r="D27" s="26"/>
+      <c r="E27" s="26"/>
+      <c r="F27" s="26"/>
+      <c r="G27" s="26"/>
+      <c r="H27" s="26"/>
+      <c r="I27" s="24"/>
+      <c r="J27" s="88"/>
+      <c r="K27" s="104"/>
+      <c r="L27" s="105"/>
+      <c r="M27" s="113"/>
     </row>
     <row r="28" spans="1:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="31"/>
-      <c r="C28" s="30"/>
-      <c r="D28" s="30"/>
-      <c r="E28" s="30"/>
-      <c r="F28" s="30"/>
-      <c r="G28" s="30"/>
-      <c r="H28" s="30"/>
-      <c r="I28" s="30"/>
-      <c r="J28" s="29"/>
-      <c r="K28" s="75"/>
-      <c r="L28" s="76"/>
-      <c r="M28" s="28"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="24"/>
+      <c r="D28" s="24"/>
+      <c r="E28" s="24"/>
+      <c r="F28" s="87"/>
+      <c r="G28" s="87"/>
+      <c r="H28" s="87"/>
+      <c r="I28" s="24"/>
+      <c r="J28" s="23"/>
+      <c r="K28" s="104"/>
+      <c r="L28" s="105"/>
+      <c r="M28" s="113"/>
     </row>
     <row r="29" spans="1:13" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="77"/>
-      <c r="C29" s="71"/>
-      <c r="D29" s="71"/>
-      <c r="E29" s="71"/>
-      <c r="F29" s="71"/>
-      <c r="G29" s="71"/>
-      <c r="H29" s="69"/>
-      <c r="I29" s="71"/>
-      <c r="J29" s="72"/>
-      <c r="K29" s="78">
-        <f>+K27*10/100</f>
-        <v>0</v>
-      </c>
-      <c r="L29" s="79"/>
-      <c r="M29" s="28">
-        <f>+M27*10%</f>
-        <v>0</v>
-      </c>
+      <c r="B29" s="30"/>
+      <c r="C29" s="95"/>
+      <c r="D29" s="95"/>
+      <c r="E29" s="95"/>
+      <c r="F29" s="95"/>
+      <c r="G29" s="95"/>
+      <c r="H29" s="83"/>
+      <c r="I29" s="87"/>
+      <c r="J29" s="88"/>
+      <c r="K29" s="106"/>
+      <c r="L29" s="107"/>
+      <c r="M29" s="113"/>
     </row>
     <row r="30" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="27"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="5"/>
-      <c r="G30" s="5"/>
+      <c r="B30" s="96"/>
+      <c r="C30" s="94"/>
+      <c r="D30" s="94"/>
+      <c r="E30" s="97"/>
+      <c r="F30" s="97"/>
+      <c r="G30" s="94"/>
       <c r="H30" s="5"/>
       <c r="I30" s="5"/>
-      <c r="J30" s="26"/>
-      <c r="K30" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="L30" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="M30" s="9"/>
+      <c r="J30" s="22"/>
+      <c r="K30" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="L30" s="110"/>
+      <c r="M30" s="8"/>
     </row>
     <row r="31" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="25"/>
-      <c r="C31" s="17"/>
-      <c r="D31" s="17"/>
-      <c r="E31" s="24"/>
-      <c r="F31" s="24"/>
-      <c r="G31" s="24"/>
-      <c r="H31" s="24"/>
-      <c r="I31" s="24"/>
-      <c r="J31" s="23"/>
-      <c r="K31" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="L31" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="M31" s="9">
+      <c r="B31" s="98"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="99"/>
+      <c r="F31" s="99"/>
+      <c r="G31" s="99"/>
+      <c r="H31" s="99"/>
+      <c r="I31" s="21"/>
+      <c r="J31" s="100"/>
+      <c r="K31" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="L31" s="19"/>
+      <c r="M31" s="8">
         <f>+M18</f>
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B32" s="80" t="s">
-        <v>15</v>
-      </c>
-      <c r="C32" s="81"/>
-      <c r="D32" s="81"/>
-      <c r="E32" s="81"/>
-      <c r="F32" s="81"/>
-      <c r="G32" s="81"/>
-      <c r="H32" s="81"/>
-      <c r="I32" s="81"/>
-      <c r="J32" s="82"/>
-      <c r="K32" s="86" t="s">
-        <v>14</v>
-      </c>
-      <c r="L32" s="20"/>
-      <c r="M32" s="19"/>
+      <c r="B32" s="51"/>
+      <c r="C32" s="52"/>
+      <c r="D32" s="52"/>
+      <c r="E32" s="52"/>
+      <c r="F32" s="52"/>
+      <c r="G32" s="52"/>
+      <c r="H32" s="52"/>
+      <c r="I32" s="52"/>
+      <c r="J32" s="53"/>
+      <c r="K32" s="57" t="s">
+        <v>12</v>
+      </c>
+      <c r="L32" s="18"/>
+      <c r="M32" s="17"/>
     </row>
     <row r="33" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="18"/>
-      <c r="B33" s="83"/>
-      <c r="C33" s="84"/>
-      <c r="D33" s="84"/>
-      <c r="E33" s="84"/>
-      <c r="F33" s="84"/>
-      <c r="G33" s="84"/>
-      <c r="H33" s="84"/>
-      <c r="I33" s="84"/>
-      <c r="J33" s="85"/>
-      <c r="K33" s="87"/>
-      <c r="L33" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="M33" s="16">
+      <c r="A33" s="16"/>
+      <c r="B33" s="54"/>
+      <c r="C33" s="55"/>
+      <c r="D33" s="55"/>
+      <c r="E33" s="55"/>
+      <c r="F33" s="55"/>
+      <c r="G33" s="55"/>
+      <c r="H33" s="55"/>
+      <c r="I33" s="55"/>
+      <c r="J33" s="56"/>
+      <c r="K33" s="58"/>
+      <c r="L33" s="15"/>
+      <c r="M33" s="14">
         <f>+M22+M21</f>
         <v>0</v>
       </c>
-      <c r="P33" s="15"/>
+      <c r="P33" s="13"/>
     </row>
     <row r="34" spans="1:16" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B34" s="88" t="s">
-        <v>13</v>
-      </c>
-      <c r="C34" s="89"/>
-      <c r="D34" s="89"/>
-      <c r="E34" s="89"/>
-      <c r="F34" s="89"/>
-      <c r="G34" s="89"/>
-      <c r="H34" s="89"/>
-      <c r="I34" s="89"/>
-      <c r="J34" s="90"/>
-      <c r="K34" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="L34" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="M34" s="9">
+      <c r="B34" s="59"/>
+      <c r="C34" s="60"/>
+      <c r="D34" s="60"/>
+      <c r="E34" s="60"/>
+      <c r="F34" s="60"/>
+      <c r="G34" s="60"/>
+      <c r="H34" s="60"/>
+      <c r="I34" s="60"/>
+      <c r="J34" s="61"/>
+      <c r="K34" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="L34" s="11"/>
+      <c r="M34" s="8">
         <f>+M30+M31+M33</f>
         <v>0</v>
       </c>
-      <c r="P34" s="12"/>
+      <c r="P34" s="10"/>
     </row>
     <row r="35" spans="1:16" ht="6.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B35" s="91"/>
-      <c r="C35" s="92"/>
-      <c r="D35" s="92"/>
-      <c r="E35" s="92"/>
-      <c r="F35" s="92"/>
-      <c r="G35" s="92"/>
-      <c r="H35" s="92"/>
-      <c r="I35" s="92"/>
-      <c r="J35" s="93"/>
-      <c r="K35" s="94" t="s">
-        <v>11</v>
-      </c>
-      <c r="L35" s="96" t="s">
+      <c r="B35" s="62"/>
+      <c r="C35" s="63"/>
+      <c r="D35" s="63"/>
+      <c r="E35" s="63"/>
+      <c r="F35" s="63"/>
+      <c r="G35" s="63"/>
+      <c r="H35" s="63"/>
+      <c r="I35" s="63"/>
+      <c r="J35" s="64"/>
+      <c r="K35" s="65" t="s">
+        <v>10</v>
+      </c>
+      <c r="L35" s="67"/>
+      <c r="M35" s="116"/>
+      <c r="O35" s="69" t="s">
+        <v>9</v>
+      </c>
+      <c r="P35" s="70"/>
+    </row>
+    <row r="36" spans="1:16" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B36" s="76" t="s">
+        <v>8</v>
+      </c>
+      <c r="C36" s="77"/>
+      <c r="D36" s="77"/>
+      <c r="E36" s="77"/>
+      <c r="F36" s="77"/>
+      <c r="G36" s="77"/>
+      <c r="H36" s="77"/>
+      <c r="I36" s="77"/>
+      <c r="J36" s="78"/>
+      <c r="K36" s="66"/>
+      <c r="L36" s="68"/>
+      <c r="M36" s="116"/>
+      <c r="O36" s="69"/>
+      <c r="P36" s="70"/>
+    </row>
+    <row r="37" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B37" s="79"/>
+      <c r="C37" s="80"/>
+      <c r="D37" s="80"/>
+      <c r="E37" s="80"/>
+      <c r="F37" s="80"/>
+      <c r="G37" s="80"/>
+      <c r="H37" s="80"/>
+      <c r="I37" s="80"/>
+      <c r="J37" s="81"/>
+      <c r="K37" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="M35" s="98"/>
-      <c r="O35" s="99" t="s">
-        <v>10</v>
-      </c>
-      <c r="P35" s="100"/>
-    </row>
-    <row r="36" spans="1:16" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B36" s="101" t="s">
-        <v>9</v>
-      </c>
-      <c r="C36" s="102"/>
-      <c r="D36" s="102"/>
-      <c r="E36" s="102"/>
-      <c r="F36" s="102"/>
-      <c r="G36" s="102"/>
-      <c r="H36" s="102"/>
-      <c r="I36" s="102"/>
-      <c r="J36" s="103"/>
-      <c r="K36" s="95"/>
-      <c r="L36" s="97"/>
-      <c r="M36" s="98"/>
-      <c r="O36" s="99"/>
-      <c r="P36" s="100"/>
-    </row>
-    <row r="37" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B37" s="104"/>
-      <c r="C37" s="105"/>
-      <c r="D37" s="105"/>
-      <c r="E37" s="105"/>
-      <c r="F37" s="105"/>
-      <c r="G37" s="105"/>
-      <c r="H37" s="105"/>
-      <c r="I37" s="105"/>
-      <c r="J37" s="106"/>
-      <c r="K37" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="L37" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="M37" s="9">
+      <c r="L37" s="9"/>
+      <c r="M37" s="8">
         <f>+M34+M35</f>
         <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="B38" s="8" t="s">
+      <c r="B38" s="114" t="s">
         <v>6</v>
       </c>
-      <c r="C38" s="6"/>
-      <c r="D38" s="6"/>
-      <c r="E38" s="6"/>
-      <c r="F38" s="6"/>
-      <c r="G38" s="6"/>
-      <c r="H38" s="6"/>
-      <c r="I38" s="6"/>
-      <c r="J38" s="6"/>
+      <c r="C38" s="115"/>
+      <c r="D38" s="115"/>
+      <c r="E38" s="115"/>
+      <c r="F38" s="115"/>
+      <c r="G38" s="115"/>
+      <c r="H38" s="115"/>
+      <c r="I38" s="115"/>
+      <c r="J38" s="115"/>
       <c r="K38" s="6"/>
       <c r="L38" s="6"/>
       <c r="M38" s="6"/>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="B39" s="6"/>
-      <c r="C39" s="6"/>
-      <c r="D39" s="6"/>
-      <c r="E39" s="6"/>
-      <c r="F39" s="6"/>
-      <c r="G39" s="6"/>
-      <c r="H39" s="6"/>
-      <c r="I39" s="6"/>
-      <c r="J39" s="6"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
+      <c r="J39" s="2"/>
       <c r="K39" s="6"/>
       <c r="L39" s="6"/>
       <c r="M39" s="6"/>
@@ -1920,24 +1893,24 @@
       <c r="M41" s="7"/>
     </row>
     <row r="42" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B42" s="107" t="s">
+      <c r="B42" s="71" t="s">
         <v>5</v>
       </c>
-      <c r="C42" s="107"/>
-      <c r="D42" s="107"/>
-      <c r="E42" s="107"/>
-      <c r="F42" s="107"/>
+      <c r="C42" s="71"/>
+      <c r="D42" s="71"/>
+      <c r="E42" s="71"/>
+      <c r="F42" s="71"/>
       <c r="G42" s="6"/>
-      <c r="H42" s="108" t="s">
+      <c r="H42" s="72" t="s">
         <v>4</v>
       </c>
-      <c r="I42" s="108"/>
-      <c r="J42" s="108"/>
+      <c r="I42" s="72"/>
+      <c r="J42" s="72"/>
       <c r="K42" s="5"/>
-      <c r="L42" s="109" t="s">
+      <c r="L42" s="73" t="s">
         <v>3</v>
       </c>
-      <c r="M42" s="109"/>
+      <c r="M42" s="73"/>
       <c r="N42" s="4"/>
       <c r="O42" s="4"/>
       <c r="P42" s="4"/>
@@ -1949,81 +1922,80 @@
       <c r="E43" s="2"/>
       <c r="F43" s="2"/>
       <c r="G43" s="3"/>
-      <c r="H43" s="108"/>
-      <c r="I43" s="108"/>
-      <c r="J43" s="108"/>
+      <c r="H43" s="72"/>
+      <c r="I43" s="72"/>
+      <c r="J43" s="72"/>
       <c r="K43" s="2"/>
       <c r="L43" s="2"/>
       <c r="M43" s="2"/>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="B44" s="110"/>
-      <c r="C44" s="110"/>
-      <c r="D44" s="110"/>
-      <c r="E44" s="110"/>
-      <c r="F44" s="110"/>
-      <c r="G44" s="110"/>
-      <c r="H44" s="110"/>
-      <c r="I44" s="110"/>
-      <c r="J44" s="110"/>
-      <c r="K44" s="110"/>
-      <c r="L44" s="110"/>
-      <c r="M44" s="110"/>
+      <c r="B44" s="74"/>
+      <c r="C44" s="74"/>
+      <c r="D44" s="74"/>
+      <c r="E44" s="74"/>
+      <c r="F44" s="74"/>
+      <c r="G44" s="74"/>
+      <c r="H44" s="74"/>
+      <c r="I44" s="74"/>
+      <c r="J44" s="74"/>
+      <c r="K44" s="74"/>
+      <c r="L44" s="74"/>
+      <c r="M44" s="74"/>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="B45" s="60" t="s">
+      <c r="B45" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="C45" s="60"/>
-      <c r="D45" s="60"/>
-      <c r="E45" s="60"/>
-      <c r="F45" s="60"/>
-      <c r="G45" s="60"/>
-      <c r="H45" s="60"/>
-      <c r="I45" s="60"/>
-      <c r="J45" s="60"/>
-      <c r="K45" s="60"/>
-      <c r="L45" s="60"/>
-      <c r="M45" s="60"/>
+      <c r="C45" s="48"/>
+      <c r="D45" s="48"/>
+      <c r="E45" s="48"/>
+      <c r="F45" s="48"/>
+      <c r="G45" s="48"/>
+      <c r="H45" s="48"/>
+      <c r="I45" s="48"/>
+      <c r="J45" s="48"/>
+      <c r="K45" s="48"/>
+      <c r="L45" s="48"/>
+      <c r="M45" s="48"/>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="B46" s="60" t="s">
+      <c r="B46" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="C46" s="60"/>
-      <c r="D46" s="60"/>
-      <c r="E46" s="60"/>
-      <c r="F46" s="60"/>
-      <c r="G46" s="60"/>
-      <c r="H46" s="60"/>
-      <c r="I46" s="60"/>
-      <c r="J46" s="60"/>
-      <c r="K46" s="60"/>
-      <c r="L46" s="60"/>
-      <c r="M46" s="60"/>
+      <c r="C46" s="48"/>
+      <c r="D46" s="48"/>
+      <c r="E46" s="48"/>
+      <c r="F46" s="48"/>
+      <c r="G46" s="48"/>
+      <c r="H46" s="48"/>
+      <c r="I46" s="48"/>
+      <c r="J46" s="48"/>
+      <c r="K46" s="48"/>
+      <c r="L46" s="48"/>
+      <c r="M46" s="48"/>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="B47" s="60" t="s">
+      <c r="B47" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="C47" s="60"/>
-      <c r="D47" s="60"/>
-      <c r="E47" s="60"/>
-      <c r="F47" s="60"/>
-      <c r="G47" s="60"/>
-      <c r="H47" s="60"/>
-      <c r="I47" s="60"/>
-      <c r="J47" s="60"/>
-      <c r="K47" s="60"/>
-      <c r="L47" s="60"/>
-      <c r="M47" s="60"/>
+      <c r="C47" s="48"/>
+      <c r="D47" s="48"/>
+      <c r="E47" s="48"/>
+      <c r="F47" s="48"/>
+      <c r="G47" s="48"/>
+      <c r="H47" s="48"/>
+      <c r="I47" s="48"/>
+      <c r="J47" s="48"/>
+      <c r="K47" s="48"/>
+      <c r="L47" s="48"/>
+      <c r="M47" s="48"/>
     </row>
   </sheetData>
-  <mergeCells count="52">
+  <mergeCells count="27">
     <mergeCell ref="M35:M36"/>
     <mergeCell ref="O35:O36"/>
     <mergeCell ref="P35:P36"/>
-    <mergeCell ref="B36:J37"/>
     <mergeCell ref="B47:M47"/>
     <mergeCell ref="B42:F42"/>
     <mergeCell ref="H42:J43"/>
@@ -2036,29 +2008,6 @@
     <mergeCell ref="B34:J35"/>
     <mergeCell ref="K35:K36"/>
     <mergeCell ref="L35:L36"/>
-    <mergeCell ref="K26:L26"/>
-    <mergeCell ref="K27:L27"/>
-    <mergeCell ref="K28:L28"/>
-    <mergeCell ref="B29:G29"/>
-    <mergeCell ref="H29:J29"/>
-    <mergeCell ref="K29:L29"/>
-    <mergeCell ref="C23:J23"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="C24:J24"/>
-    <mergeCell ref="K24:L24"/>
-    <mergeCell ref="C25:J25"/>
-    <mergeCell ref="K25:L25"/>
-    <mergeCell ref="C20:J20"/>
-    <mergeCell ref="K20:L20"/>
-    <mergeCell ref="C21:J21"/>
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="C22:J22"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="B17:J18"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="C19:J19"/>
-    <mergeCell ref="K19:L19"/>
     <mergeCell ref="C12:I12"/>
     <mergeCell ref="M12:M13"/>
     <mergeCell ref="B13:C13"/>
@@ -2067,7 +2016,6 @@
     <mergeCell ref="K16:L16"/>
     <mergeCell ref="B5:J5"/>
     <mergeCell ref="B6:J6"/>
-    <mergeCell ref="C10:F10"/>
     <mergeCell ref="I10:J10"/>
     <mergeCell ref="M10:M11"/>
     <mergeCell ref="B11:D11"/>

</xml_diff>